<commit_message>
jn: actualizacion bases + nueva distribución
</commit_message>
<xml_diff>
--- a/02_Bases de Datos 2025/Judicatura/CJ 0936 Causas Art 247 corte agosto 2024(1).xlsx
+++ b/02_Bases de Datos 2025/Judicatura/CJ 0936 Causas Art 247 corte agosto 2024(1).xlsx
@@ -1189,7 +1189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1214,6 +1214,11 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -1224,7 +1229,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1235,6 +1240,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF44546A"/>
         <bgColor rgb="FF44546A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1270,7 +1281,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1287,11 +1298,14 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1834,27 +1848,46 @@
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="10">
         <v>43709.0</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="B10" s="6" t="s">
@@ -1995,50 +2028,88 @@
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="10">
         <v>43735.0</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="F16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="H16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="10">
         <v>43854.0</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="B18" s="6" t="s">
@@ -4686,119 +4757,214 @@
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="B133" s="6" t="s">
+      <c r="A133" s="8"/>
+      <c r="B133" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C133" s="7">
+      <c r="C133" s="10">
         <v>44574.0</v>
       </c>
-      <c r="D133" s="6" t="s">
+      <c r="D133" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E133" s="6" t="s">
+      <c r="E133" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F133" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G133" s="6" t="s">
+      <c r="F133" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G133" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H133" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="H133" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" s="8"/>
+      <c r="J133" s="8"/>
+      <c r="K133" s="8"/>
+      <c r="L133" s="8"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="8"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="Q133" s="8"/>
+      <c r="R133" s="8"/>
+      <c r="S133" s="8"/>
+      <c r="T133" s="8"/>
+      <c r="U133" s="8"/>
+      <c r="V133" s="8"/>
+      <c r="W133" s="8"/>
+      <c r="X133" s="8"/>
+      <c r="Y133" s="8"/>
+      <c r="Z133" s="8"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="B134" s="6" t="s">
+      <c r="A134" s="8"/>
+      <c r="B134" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C134" s="7">
+      <c r="C134" s="10">
         <v>43708.0</v>
       </c>
-      <c r="D134" s="6" t="s">
+      <c r="D134" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E134" s="6" t="s">
+      <c r="E134" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F134" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G134" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H134" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F134" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G134" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H134" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" s="8"/>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8"/>
+      <c r="M134" s="8"/>
+      <c r="N134" s="8"/>
+      <c r="O134" s="8"/>
+      <c r="P134" s="8"/>
+      <c r="Q134" s="8"/>
+      <c r="R134" s="8"/>
+      <c r="S134" s="8"/>
+      <c r="T134" s="8"/>
+      <c r="U134" s="8"/>
+      <c r="V134" s="8"/>
+      <c r="W134" s="8"/>
+      <c r="X134" s="8"/>
+      <c r="Y134" s="8"/>
+      <c r="Z134" s="8"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="B135" s="6" t="s">
+      <c r="A135" s="8"/>
+      <c r="B135" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C135" s="7">
+      <c r="C135" s="10">
         <v>43708.0</v>
       </c>
-      <c r="D135" s="6" t="s">
+      <c r="D135" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E135" s="6" t="s">
+      <c r="E135" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F135" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G135" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H135" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F135" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G135" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H135" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="8"/>
+      <c r="L135" s="8"/>
+      <c r="M135" s="8"/>
+      <c r="N135" s="8"/>
+      <c r="O135" s="8"/>
+      <c r="P135" s="8"/>
+      <c r="Q135" s="8"/>
+      <c r="R135" s="8"/>
+      <c r="S135" s="8"/>
+      <c r="T135" s="8"/>
+      <c r="U135" s="8"/>
+      <c r="V135" s="8"/>
+      <c r="W135" s="8"/>
+      <c r="X135" s="8"/>
+      <c r="Y135" s="8"/>
+      <c r="Z135" s="8"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="B136" s="6" t="s">
+      <c r="A136" s="8"/>
+      <c r="B136" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C136" s="7">
+      <c r="C136" s="10">
         <v>45458.0</v>
       </c>
-      <c r="D136" s="6" t="s">
+      <c r="D136" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E136" s="6" t="s">
+      <c r="E136" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="F136" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G136" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H136" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F136" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G136" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H136" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" s="8"/>
+      <c r="J136" s="8"/>
+      <c r="K136" s="8"/>
+      <c r="L136" s="8"/>
+      <c r="M136" s="8"/>
+      <c r="N136" s="8"/>
+      <c r="O136" s="8"/>
+      <c r="P136" s="8"/>
+      <c r="Q136" s="8"/>
+      <c r="R136" s="8"/>
+      <c r="S136" s="8"/>
+      <c r="T136" s="8"/>
+      <c r="U136" s="8"/>
+      <c r="V136" s="8"/>
+      <c r="W136" s="8"/>
+      <c r="X136" s="8"/>
+      <c r="Y136" s="8"/>
+      <c r="Z136" s="8"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="B137" s="6" t="s">
+      <c r="A137" s="8"/>
+      <c r="B137" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C137" s="7">
+      <c r="C137" s="10">
         <v>43642.0</v>
       </c>
-      <c r="D137" s="6" t="s">
+      <c r="D137" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E137" s="6" t="s">
+      <c r="E137" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F137" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G137" s="6" t="s">
+      <c r="F137" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G137" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="H137" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="H137" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" s="8"/>
+      <c r="J137" s="8"/>
+      <c r="K137" s="8"/>
+      <c r="L137" s="8"/>
+      <c r="M137" s="8"/>
+      <c r="N137" s="8"/>
+      <c r="O137" s="8"/>
+      <c r="P137" s="8"/>
+      <c r="Q137" s="8"/>
+      <c r="R137" s="8"/>
+      <c r="S137" s="8"/>
+      <c r="T137" s="8"/>
+      <c r="U137" s="8"/>
+      <c r="V137" s="8"/>
+      <c r="W137" s="8"/>
+      <c r="X137" s="8"/>
+      <c r="Y137" s="8"/>
+      <c r="Z137" s="8"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
       <c r="B138" s="6" t="s">
@@ -4824,27 +4990,46 @@
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="B139" s="6" t="s">
+      <c r="A139" s="8"/>
+      <c r="B139" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C139" s="7">
+      <c r="C139" s="10">
         <v>45334.0</v>
       </c>
-      <c r="D139" s="6" t="s">
+      <c r="D139" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E139" s="6" t="s">
+      <c r="E139" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F139" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G139" s="6" t="s">
+      <c r="F139" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G139" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H139" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="H139" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" s="8"/>
+      <c r="J139" s="8"/>
+      <c r="K139" s="8"/>
+      <c r="L139" s="8"/>
+      <c r="M139" s="8"/>
+      <c r="N139" s="8"/>
+      <c r="O139" s="8"/>
+      <c r="P139" s="8"/>
+      <c r="Q139" s="8"/>
+      <c r="R139" s="8"/>
+      <c r="S139" s="8"/>
+      <c r="T139" s="8"/>
+      <c r="U139" s="8"/>
+      <c r="V139" s="8"/>
+      <c r="W139" s="8"/>
+      <c r="X139" s="8"/>
+      <c r="Y139" s="8"/>
+      <c r="Z139" s="8"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="B140" s="6" t="s">
@@ -4962,73 +5147,130 @@
       </c>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="B145" s="6" t="s">
+      <c r="A145" s="8"/>
+      <c r="B145" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C145" s="7">
+      <c r="C145" s="10">
         <v>44284.0</v>
       </c>
-      <c r="D145" s="6" t="s">
+      <c r="D145" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E145" s="6" t="s">
+      <c r="E145" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F145" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G145" s="6" t="s">
+      <c r="F145" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G145" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H145" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="H145" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" s="8"/>
+      <c r="J145" s="8"/>
+      <c r="K145" s="8"/>
+      <c r="L145" s="8"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="8"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="8"/>
+      <c r="Q145" s="8"/>
+      <c r="R145" s="8"/>
+      <c r="S145" s="8"/>
+      <c r="T145" s="8"/>
+      <c r="U145" s="8"/>
+      <c r="V145" s="8"/>
+      <c r="W145" s="8"/>
+      <c r="X145" s="8"/>
+      <c r="Y145" s="8"/>
+      <c r="Z145" s="8"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="B146" s="6" t="s">
+      <c r="A146" s="8"/>
+      <c r="B146" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C146" s="7">
+      <c r="C146" s="10">
         <v>44246.0</v>
       </c>
-      <c r="D146" s="6" t="s">
+      <c r="D146" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E146" s="6" t="s">
+      <c r="E146" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F146" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G146" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H146" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F146" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G146" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H146" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" s="8"/>
+      <c r="J146" s="8"/>
+      <c r="K146" s="8"/>
+      <c r="L146" s="8"/>
+      <c r="M146" s="8"/>
+      <c r="N146" s="8"/>
+      <c r="O146" s="8"/>
+      <c r="P146" s="8"/>
+      <c r="Q146" s="8"/>
+      <c r="R146" s="8"/>
+      <c r="S146" s="8"/>
+      <c r="T146" s="8"/>
+      <c r="U146" s="8"/>
+      <c r="V146" s="8"/>
+      <c r="W146" s="8"/>
+      <c r="X146" s="8"/>
+      <c r="Y146" s="8"/>
+      <c r="Z146" s="8"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="B147" s="6" t="s">
+      <c r="A147" s="8"/>
+      <c r="B147" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C147" s="7">
+      <c r="C147" s="10">
         <v>44335.0</v>
       </c>
-      <c r="D147" s="6" t="s">
+      <c r="D147" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E147" s="6" t="s">
+      <c r="E147" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F147" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G147" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H147" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="F147" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G147" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H147" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" s="8"/>
+      <c r="J147" s="8"/>
+      <c r="K147" s="8"/>
+      <c r="L147" s="8"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="8"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="8"/>
+      <c r="Q147" s="8"/>
+      <c r="R147" s="8"/>
+      <c r="S147" s="8"/>
+      <c r="T147" s="8"/>
+      <c r="U147" s="8"/>
+      <c r="V147" s="8"/>
+      <c r="W147" s="8"/>
+      <c r="X147" s="8"/>
+      <c r="Y147" s="8"/>
+      <c r="Z147" s="8"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="B148" s="6" t="s">
@@ -7401,31 +7643,31 @@
     </row>
     <row r="251" ht="14.25" customHeight="1"/>
     <row r="252" ht="14.25" customHeight="1">
-      <c r="B252" s="8"/>
-      <c r="C252" s="9"/>
-      <c r="D252" s="8"/>
-      <c r="E252" s="8"/>
-      <c r="F252" s="8"/>
-      <c r="G252" s="8"/>
-      <c r="H252" s="8"/>
+      <c r="B252" s="11"/>
+      <c r="C252" s="12"/>
+      <c r="D252" s="11"/>
+      <c r="E252" s="11"/>
+      <c r="F252" s="11"/>
+      <c r="G252" s="11"/>
+      <c r="H252" s="11"/>
     </row>
     <row r="253" ht="14.25" customHeight="1">
-      <c r="B253" s="10" t="s">
+      <c r="B253" s="13" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="254" ht="14.25" customHeight="1">
-      <c r="B254" s="10" t="s">
+      <c r="B254" s="13" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="255" ht="14.25" customHeight="1">
-      <c r="B255" s="11" t="s">
+      <c r="B255" s="14" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="256" ht="14.25" customHeight="1">
-      <c r="B256" s="10"/>
+      <c r="B256" s="13"/>
     </row>
     <row r="257" ht="14.25" customHeight="1"/>
     <row r="258" ht="14.25" customHeight="1"/>
@@ -13981,31 +14223,31 @@
     <row r="203" ht="14.25" customHeight="1"/>
     <row r="204" ht="14.25" customHeight="1"/>
     <row r="205" ht="14.25" customHeight="1">
-      <c r="B205" s="8"/>
-      <c r="C205" s="9"/>
-      <c r="D205" s="8"/>
-      <c r="E205" s="8"/>
-      <c r="F205" s="8"/>
-      <c r="G205" s="8"/>
-      <c r="H205" s="8"/>
+      <c r="B205" s="11"/>
+      <c r="C205" s="12"/>
+      <c r="D205" s="11"/>
+      <c r="E205" s="11"/>
+      <c r="F205" s="11"/>
+      <c r="G205" s="11"/>
+      <c r="H205" s="11"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
-      <c r="B206" s="10" t="s">
+      <c r="B206" s="13" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="207" ht="14.25" customHeight="1">
-      <c r="B207" s="10" t="s">
+      <c r="B207" s="13" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="208" ht="14.25" customHeight="1">
-      <c r="B208" s="11" t="s">
+      <c r="B208" s="14" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="209" ht="14.25" customHeight="1">
-      <c r="B209" s="10"/>
+      <c r="B209" s="13"/>
     </row>
     <row r="210" ht="14.25" customHeight="1"/>
     <row r="211" ht="14.25" customHeight="1"/>
@@ -17724,34 +17966,34 @@
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="H115" s="12"/>
+      <c r="H115" s="15"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="B116" s="8"/>
-      <c r="C116" s="9"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
+      <c r="B116" s="11"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11"/>
+      <c r="G116" s="11"/>
+      <c r="H116" s="11"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="B117" s="10" t="s">
+      <c r="B117" s="13" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="B118" s="10" t="s">
+      <c r="B118" s="13" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="14" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="B120" s="10"/>
+      <c r="B120" s="13"/>
     </row>
     <row r="121" ht="14.25" customHeight="1"/>
     <row r="122" ht="14.25" customHeight="1"/>
@@ -17759,2629 +18001,2629 @@
     <row r="124" ht="14.25" customHeight="1"/>
     <row r="125" ht="14.25" customHeight="1"/>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="H126" s="12"/>
+      <c r="H126" s="15"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="H127" s="12"/>
+      <c r="H127" s="15"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="H128" s="12"/>
+      <c r="H128" s="15"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="H129" s="12"/>
+      <c r="H129" s="15"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="H130" s="12"/>
+      <c r="H130" s="15"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="H131" s="12"/>
+      <c r="H131" s="15"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="H132" s="12"/>
+      <c r="H132" s="15"/>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="H133" s="12"/>
+      <c r="H133" s="15"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="H134" s="12"/>
+      <c r="H134" s="15"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="H135" s="12"/>
+      <c r="H135" s="15"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="H136" s="12"/>
+      <c r="H136" s="15"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="H137" s="12"/>
+      <c r="H137" s="15"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="H138" s="12"/>
+      <c r="H138" s="15"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="H139" s="12"/>
+      <c r="H139" s="15"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="H140" s="12"/>
+      <c r="H140" s="15"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="H141" s="12"/>
+      <c r="H141" s="15"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="H142" s="12"/>
+      <c r="H142" s="15"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="H143" s="12"/>
+      <c r="H143" s="15"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="H144" s="12"/>
+      <c r="H144" s="15"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="H145" s="12"/>
+      <c r="H145" s="15"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="H146" s="12"/>
+      <c r="H146" s="15"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="H147" s="12"/>
+      <c r="H147" s="15"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="H148" s="12"/>
+      <c r="H148" s="15"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="H149" s="12"/>
+      <c r="H149" s="15"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="H150" s="12"/>
+      <c r="H150" s="15"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="H151" s="12"/>
+      <c r="H151" s="15"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="H152" s="12"/>
+      <c r="H152" s="15"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="H153" s="12"/>
+      <c r="H153" s="15"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="H154" s="12"/>
+      <c r="H154" s="15"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="H155" s="12"/>
+      <c r="H155" s="15"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="H156" s="12"/>
+      <c r="H156" s="15"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="H157" s="12"/>
+      <c r="H157" s="15"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="H158" s="12"/>
+      <c r="H158" s="15"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="H159" s="12"/>
+      <c r="H159" s="15"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="H160" s="12"/>
+      <c r="H160" s="15"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="H161" s="12"/>
+      <c r="H161" s="15"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="H162" s="12"/>
+      <c r="H162" s="15"/>
     </row>
     <row r="163" ht="14.25" customHeight="1">
-      <c r="H163" s="12"/>
+      <c r="H163" s="15"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
-      <c r="H164" s="12"/>
+      <c r="H164" s="15"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
-      <c r="H165" s="12"/>
+      <c r="H165" s="15"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
-      <c r="H166" s="12"/>
+      <c r="H166" s="15"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="H167" s="12"/>
+      <c r="H167" s="15"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
-      <c r="H168" s="12"/>
+      <c r="H168" s="15"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
-      <c r="H169" s="12"/>
+      <c r="H169" s="15"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="H170" s="12"/>
+      <c r="H170" s="15"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
-      <c r="H171" s="12"/>
+      <c r="H171" s="15"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="H172" s="12"/>
+      <c r="H172" s="15"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
-      <c r="H173" s="12"/>
+      <c r="H173" s="15"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="H174" s="12"/>
+      <c r="H174" s="15"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="H175" s="12"/>
+      <c r="H175" s="15"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="H176" s="12"/>
+      <c r="H176" s="15"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="H177" s="12"/>
+      <c r="H177" s="15"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="H178" s="12"/>
+      <c r="H178" s="15"/>
     </row>
     <row r="179" ht="14.25" customHeight="1">
-      <c r="H179" s="12"/>
+      <c r="H179" s="15"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="H180" s="12"/>
+      <c r="H180" s="15"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="H181" s="12"/>
+      <c r="H181" s="15"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
-      <c r="H182" s="12"/>
+      <c r="H182" s="15"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="H183" s="12"/>
+      <c r="H183" s="15"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
-      <c r="H184" s="12"/>
+      <c r="H184" s="15"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="H185" s="12"/>
+      <c r="H185" s="15"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="H186" s="12"/>
+      <c r="H186" s="15"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
-      <c r="H187" s="12"/>
+      <c r="H187" s="15"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="H188" s="12"/>
+      <c r="H188" s="15"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="H189" s="12"/>
+      <c r="H189" s="15"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="H190" s="12"/>
+      <c r="H190" s="15"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
-      <c r="H191" s="12"/>
+      <c r="H191" s="15"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="H192" s="12"/>
+      <c r="H192" s="15"/>
     </row>
     <row r="193" ht="14.25" customHeight="1">
-      <c r="H193" s="12"/>
+      <c r="H193" s="15"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
-      <c r="H194" s="12"/>
+      <c r="H194" s="15"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="H195" s="12"/>
+      <c r="H195" s="15"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="H196" s="12"/>
+      <c r="H196" s="15"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
-      <c r="H197" s="12"/>
+      <c r="H197" s="15"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="H198" s="12"/>
+      <c r="H198" s="15"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
-      <c r="H199" s="12"/>
+      <c r="H199" s="15"/>
     </row>
     <row r="200" ht="14.25" customHeight="1">
-      <c r="H200" s="12"/>
+      <c r="H200" s="15"/>
     </row>
     <row r="201" ht="14.25" customHeight="1">
-      <c r="H201" s="12"/>
+      <c r="H201" s="15"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
-      <c r="H202" s="12"/>
+      <c r="H202" s="15"/>
     </row>
     <row r="203" ht="14.25" customHeight="1">
-      <c r="H203" s="12"/>
+      <c r="H203" s="15"/>
     </row>
     <row r="204" ht="14.25" customHeight="1">
-      <c r="H204" s="12"/>
+      <c r="H204" s="15"/>
     </row>
     <row r="205" ht="14.25" customHeight="1">
-      <c r="H205" s="12"/>
+      <c r="H205" s="15"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
-      <c r="H206" s="12"/>
+      <c r="H206" s="15"/>
     </row>
     <row r="207" ht="14.25" customHeight="1">
-      <c r="H207" s="12"/>
+      <c r="H207" s="15"/>
     </row>
     <row r="208" ht="14.25" customHeight="1">
-      <c r="H208" s="12"/>
+      <c r="H208" s="15"/>
     </row>
     <row r="209" ht="14.25" customHeight="1">
-      <c r="H209" s="12"/>
+      <c r="H209" s="15"/>
     </row>
     <row r="210" ht="14.25" customHeight="1">
-      <c r="H210" s="12"/>
+      <c r="H210" s="15"/>
     </row>
     <row r="211" ht="14.25" customHeight="1">
-      <c r="H211" s="12"/>
+      <c r="H211" s="15"/>
     </row>
     <row r="212" ht="14.25" customHeight="1">
-      <c r="H212" s="12"/>
+      <c r="H212" s="15"/>
     </row>
     <row r="213" ht="14.25" customHeight="1">
-      <c r="H213" s="12"/>
+      <c r="H213" s="15"/>
     </row>
     <row r="214" ht="14.25" customHeight="1">
-      <c r="H214" s="12"/>
+      <c r="H214" s="15"/>
     </row>
     <row r="215" ht="14.25" customHeight="1">
-      <c r="H215" s="12"/>
+      <c r="H215" s="15"/>
     </row>
     <row r="216" ht="14.25" customHeight="1">
-      <c r="H216" s="12"/>
+      <c r="H216" s="15"/>
     </row>
     <row r="217" ht="14.25" customHeight="1">
-      <c r="H217" s="12"/>
+      <c r="H217" s="15"/>
     </row>
     <row r="218" ht="14.25" customHeight="1">
-      <c r="H218" s="12"/>
+      <c r="H218" s="15"/>
     </row>
     <row r="219" ht="14.25" customHeight="1">
-      <c r="H219" s="12"/>
+      <c r="H219" s="15"/>
     </row>
     <row r="220" ht="14.25" customHeight="1">
-      <c r="H220" s="12"/>
+      <c r="H220" s="15"/>
     </row>
     <row r="221" ht="14.25" customHeight="1">
-      <c r="H221" s="12"/>
+      <c r="H221" s="15"/>
     </row>
     <row r="222" ht="14.25" customHeight="1">
-      <c r="H222" s="12"/>
+      <c r="H222" s="15"/>
     </row>
     <row r="223" ht="14.25" customHeight="1">
-      <c r="H223" s="12"/>
+      <c r="H223" s="15"/>
     </row>
     <row r="224" ht="14.25" customHeight="1">
-      <c r="H224" s="12"/>
+      <c r="H224" s="15"/>
     </row>
     <row r="225" ht="14.25" customHeight="1">
-      <c r="H225" s="12"/>
+      <c r="H225" s="15"/>
     </row>
     <row r="226" ht="14.25" customHeight="1">
-      <c r="H226" s="12"/>
+      <c r="H226" s="15"/>
     </row>
     <row r="227" ht="14.25" customHeight="1">
-      <c r="H227" s="12"/>
+      <c r="H227" s="15"/>
     </row>
     <row r="228" ht="14.25" customHeight="1">
-      <c r="H228" s="12"/>
+      <c r="H228" s="15"/>
     </row>
     <row r="229" ht="14.25" customHeight="1">
-      <c r="H229" s="12"/>
+      <c r="H229" s="15"/>
     </row>
     <row r="230" ht="14.25" customHeight="1">
-      <c r="H230" s="12"/>
+      <c r="H230" s="15"/>
     </row>
     <row r="231" ht="14.25" customHeight="1">
-      <c r="H231" s="12"/>
+      <c r="H231" s="15"/>
     </row>
     <row r="232" ht="14.25" customHeight="1">
-      <c r="H232" s="12"/>
+      <c r="H232" s="15"/>
     </row>
     <row r="233" ht="14.25" customHeight="1">
-      <c r="H233" s="12"/>
+      <c r="H233" s="15"/>
     </row>
     <row r="234" ht="14.25" customHeight="1">
-      <c r="H234" s="12"/>
+      <c r="H234" s="15"/>
     </row>
     <row r="235" ht="14.25" customHeight="1">
-      <c r="H235" s="12"/>
+      <c r="H235" s="15"/>
     </row>
     <row r="236" ht="14.25" customHeight="1">
-      <c r="H236" s="12"/>
+      <c r="H236" s="15"/>
     </row>
     <row r="237" ht="14.25" customHeight="1">
-      <c r="H237" s="12"/>
+      <c r="H237" s="15"/>
     </row>
     <row r="238" ht="14.25" customHeight="1">
-      <c r="H238" s="12"/>
+      <c r="H238" s="15"/>
     </row>
     <row r="239" ht="14.25" customHeight="1">
-      <c r="H239" s="12"/>
+      <c r="H239" s="15"/>
     </row>
     <row r="240" ht="14.25" customHeight="1">
-      <c r="H240" s="12"/>
+      <c r="H240" s="15"/>
     </row>
     <row r="241" ht="14.25" customHeight="1">
-      <c r="H241" s="12"/>
+      <c r="H241" s="15"/>
     </row>
     <row r="242" ht="14.25" customHeight="1">
-      <c r="H242" s="12"/>
+      <c r="H242" s="15"/>
     </row>
     <row r="243" ht="14.25" customHeight="1">
-      <c r="H243" s="12"/>
+      <c r="H243" s="15"/>
     </row>
     <row r="244" ht="14.25" customHeight="1">
-      <c r="H244" s="12"/>
+      <c r="H244" s="15"/>
     </row>
     <row r="245" ht="14.25" customHeight="1">
-      <c r="H245" s="12"/>
+      <c r="H245" s="15"/>
     </row>
     <row r="246" ht="14.25" customHeight="1">
-      <c r="H246" s="12"/>
+      <c r="H246" s="15"/>
     </row>
     <row r="247" ht="14.25" customHeight="1">
-      <c r="H247" s="12"/>
+      <c r="H247" s="15"/>
     </row>
     <row r="248" ht="14.25" customHeight="1">
-      <c r="H248" s="12"/>
+      <c r="H248" s="15"/>
     </row>
     <row r="249" ht="14.25" customHeight="1">
-      <c r="H249" s="12"/>
+      <c r="H249" s="15"/>
     </row>
     <row r="250" ht="14.25" customHeight="1">
-      <c r="H250" s="12"/>
+      <c r="H250" s="15"/>
     </row>
     <row r="251" ht="14.25" customHeight="1">
-      <c r="H251" s="12"/>
+      <c r="H251" s="15"/>
     </row>
     <row r="252" ht="14.25" customHeight="1">
-      <c r="H252" s="12"/>
+      <c r="H252" s="15"/>
     </row>
     <row r="253" ht="14.25" customHeight="1">
-      <c r="H253" s="12"/>
+      <c r="H253" s="15"/>
     </row>
     <row r="254" ht="14.25" customHeight="1">
-      <c r="H254" s="12"/>
+      <c r="H254" s="15"/>
     </row>
     <row r="255" ht="14.25" customHeight="1">
-      <c r="H255" s="12"/>
+      <c r="H255" s="15"/>
     </row>
     <row r="256" ht="14.25" customHeight="1">
-      <c r="H256" s="12"/>
+      <c r="H256" s="15"/>
     </row>
     <row r="257" ht="14.25" customHeight="1">
-      <c r="H257" s="12"/>
+      <c r="H257" s="15"/>
     </row>
     <row r="258" ht="14.25" customHeight="1">
-      <c r="H258" s="12"/>
+      <c r="H258" s="15"/>
     </row>
     <row r="259" ht="14.25" customHeight="1">
-      <c r="H259" s="12"/>
+      <c r="H259" s="15"/>
     </row>
     <row r="260" ht="14.25" customHeight="1">
-      <c r="H260" s="12"/>
+      <c r="H260" s="15"/>
     </row>
     <row r="261" ht="14.25" customHeight="1">
-      <c r="H261" s="12"/>
+      <c r="H261" s="15"/>
     </row>
     <row r="262" ht="14.25" customHeight="1">
-      <c r="H262" s="12"/>
+      <c r="H262" s="15"/>
     </row>
     <row r="263" ht="14.25" customHeight="1">
-      <c r="H263" s="12"/>
+      <c r="H263" s="15"/>
     </row>
     <row r="264" ht="14.25" customHeight="1">
-      <c r="H264" s="12"/>
+      <c r="H264" s="15"/>
     </row>
     <row r="265" ht="14.25" customHeight="1">
-      <c r="H265" s="12"/>
+      <c r="H265" s="15"/>
     </row>
     <row r="266" ht="14.25" customHeight="1">
-      <c r="H266" s="12"/>
+      <c r="H266" s="15"/>
     </row>
     <row r="267" ht="14.25" customHeight="1">
-      <c r="H267" s="12"/>
+      <c r="H267" s="15"/>
     </row>
     <row r="268" ht="14.25" customHeight="1">
-      <c r="H268" s="12"/>
+      <c r="H268" s="15"/>
     </row>
     <row r="269" ht="14.25" customHeight="1">
-      <c r="H269" s="12"/>
+      <c r="H269" s="15"/>
     </row>
     <row r="270" ht="14.25" customHeight="1">
-      <c r="H270" s="12"/>
+      <c r="H270" s="15"/>
     </row>
     <row r="271" ht="14.25" customHeight="1">
-      <c r="H271" s="12"/>
+      <c r="H271" s="15"/>
     </row>
     <row r="272" ht="14.25" customHeight="1">
-      <c r="H272" s="12"/>
+      <c r="H272" s="15"/>
     </row>
     <row r="273" ht="14.25" customHeight="1">
-      <c r="H273" s="12"/>
+      <c r="H273" s="15"/>
     </row>
     <row r="274" ht="14.25" customHeight="1">
-      <c r="H274" s="12"/>
+      <c r="H274" s="15"/>
     </row>
     <row r="275" ht="14.25" customHeight="1">
-      <c r="H275" s="12"/>
+      <c r="H275" s="15"/>
     </row>
     <row r="276" ht="14.25" customHeight="1">
-      <c r="H276" s="12"/>
+      <c r="H276" s="15"/>
     </row>
     <row r="277" ht="14.25" customHeight="1">
-      <c r="H277" s="12"/>
+      <c r="H277" s="15"/>
     </row>
     <row r="278" ht="14.25" customHeight="1">
-      <c r="H278" s="12"/>
+      <c r="H278" s="15"/>
     </row>
     <row r="279" ht="14.25" customHeight="1">
-      <c r="H279" s="12"/>
+      <c r="H279" s="15"/>
     </row>
     <row r="280" ht="14.25" customHeight="1">
-      <c r="H280" s="12"/>
+      <c r="H280" s="15"/>
     </row>
     <row r="281" ht="14.25" customHeight="1">
-      <c r="H281" s="12"/>
+      <c r="H281" s="15"/>
     </row>
     <row r="282" ht="14.25" customHeight="1">
-      <c r="H282" s="12"/>
+      <c r="H282" s="15"/>
     </row>
     <row r="283" ht="14.25" customHeight="1">
-      <c r="H283" s="12"/>
+      <c r="H283" s="15"/>
     </row>
     <row r="284" ht="14.25" customHeight="1">
-      <c r="H284" s="12"/>
+      <c r="H284" s="15"/>
     </row>
     <row r="285" ht="14.25" customHeight="1">
-      <c r="H285" s="12"/>
+      <c r="H285" s="15"/>
     </row>
     <row r="286" ht="14.25" customHeight="1">
-      <c r="H286" s="12"/>
+      <c r="H286" s="15"/>
     </row>
     <row r="287" ht="14.25" customHeight="1">
-      <c r="H287" s="12"/>
+      <c r="H287" s="15"/>
     </row>
     <row r="288" ht="14.25" customHeight="1">
-      <c r="H288" s="12"/>
+      <c r="H288" s="15"/>
     </row>
     <row r="289" ht="14.25" customHeight="1">
-      <c r="H289" s="12"/>
+      <c r="H289" s="15"/>
     </row>
     <row r="290" ht="14.25" customHeight="1">
-      <c r="H290" s="12"/>
+      <c r="H290" s="15"/>
     </row>
     <row r="291" ht="14.25" customHeight="1">
-      <c r="H291" s="12"/>
+      <c r="H291" s="15"/>
     </row>
     <row r="292" ht="14.25" customHeight="1">
-      <c r="H292" s="12"/>
+      <c r="H292" s="15"/>
     </row>
     <row r="293" ht="14.25" customHeight="1">
-      <c r="H293" s="12"/>
+      <c r="H293" s="15"/>
     </row>
     <row r="294" ht="14.25" customHeight="1">
-      <c r="H294" s="12"/>
+      <c r="H294" s="15"/>
     </row>
     <row r="295" ht="14.25" customHeight="1">
-      <c r="H295" s="12"/>
+      <c r="H295" s="15"/>
     </row>
     <row r="296" ht="14.25" customHeight="1">
-      <c r="H296" s="12"/>
+      <c r="H296" s="15"/>
     </row>
     <row r="297" ht="14.25" customHeight="1">
-      <c r="H297" s="12"/>
+      <c r="H297" s="15"/>
     </row>
     <row r="298" ht="14.25" customHeight="1">
-      <c r="H298" s="12"/>
+      <c r="H298" s="15"/>
     </row>
     <row r="299" ht="14.25" customHeight="1">
-      <c r="H299" s="12"/>
+      <c r="H299" s="15"/>
     </row>
     <row r="300" ht="14.25" customHeight="1">
-      <c r="H300" s="12"/>
+      <c r="H300" s="15"/>
     </row>
     <row r="301" ht="14.25" customHeight="1">
-      <c r="H301" s="12"/>
+      <c r="H301" s="15"/>
     </row>
     <row r="302" ht="14.25" customHeight="1">
-      <c r="H302" s="12"/>
+      <c r="H302" s="15"/>
     </row>
     <row r="303" ht="14.25" customHeight="1">
-      <c r="H303" s="12"/>
+      <c r="H303" s="15"/>
     </row>
     <row r="304" ht="14.25" customHeight="1">
-      <c r="H304" s="12"/>
+      <c r="H304" s="15"/>
     </row>
     <row r="305" ht="14.25" customHeight="1">
-      <c r="H305" s="12"/>
+      <c r="H305" s="15"/>
     </row>
     <row r="306" ht="14.25" customHeight="1">
-      <c r="H306" s="12"/>
+      <c r="H306" s="15"/>
     </row>
     <row r="307" ht="14.25" customHeight="1">
-      <c r="H307" s="12"/>
+      <c r="H307" s="15"/>
     </row>
     <row r="308" ht="14.25" customHeight="1">
-      <c r="H308" s="12"/>
+      <c r="H308" s="15"/>
     </row>
     <row r="309" ht="14.25" customHeight="1">
-      <c r="H309" s="12"/>
+      <c r="H309" s="15"/>
     </row>
     <row r="310" ht="14.25" customHeight="1">
-      <c r="H310" s="12"/>
+      <c r="H310" s="15"/>
     </row>
     <row r="311" ht="14.25" customHeight="1">
-      <c r="H311" s="12"/>
+      <c r="H311" s="15"/>
     </row>
     <row r="312" ht="14.25" customHeight="1">
-      <c r="H312" s="12"/>
+      <c r="H312" s="15"/>
     </row>
     <row r="313" ht="14.25" customHeight="1">
-      <c r="H313" s="12"/>
+      <c r="H313" s="15"/>
     </row>
     <row r="314" ht="14.25" customHeight="1">
-      <c r="H314" s="12"/>
+      <c r="H314" s="15"/>
     </row>
     <row r="315" ht="14.25" customHeight="1">
-      <c r="H315" s="12"/>
+      <c r="H315" s="15"/>
     </row>
     <row r="316" ht="14.25" customHeight="1">
-      <c r="H316" s="12"/>
+      <c r="H316" s="15"/>
     </row>
     <row r="317" ht="14.25" customHeight="1">
-      <c r="H317" s="12"/>
+      <c r="H317" s="15"/>
     </row>
     <row r="318" ht="14.25" customHeight="1">
-      <c r="H318" s="12"/>
+      <c r="H318" s="15"/>
     </row>
     <row r="319" ht="14.25" customHeight="1">
-      <c r="H319" s="12"/>
+      <c r="H319" s="15"/>
     </row>
     <row r="320" ht="14.25" customHeight="1">
-      <c r="H320" s="12"/>
+      <c r="H320" s="15"/>
     </row>
     <row r="321" ht="14.25" customHeight="1">
-      <c r="H321" s="12"/>
+      <c r="H321" s="15"/>
     </row>
     <row r="322" ht="14.25" customHeight="1">
-      <c r="H322" s="12"/>
+      <c r="H322" s="15"/>
     </row>
     <row r="323" ht="14.25" customHeight="1">
-      <c r="H323" s="12"/>
+      <c r="H323" s="15"/>
     </row>
     <row r="324" ht="14.25" customHeight="1">
-      <c r="H324" s="12"/>
+      <c r="H324" s="15"/>
     </row>
     <row r="325" ht="14.25" customHeight="1">
-      <c r="H325" s="12"/>
+      <c r="H325" s="15"/>
     </row>
     <row r="326" ht="14.25" customHeight="1">
-      <c r="H326" s="12"/>
+      <c r="H326" s="15"/>
     </row>
     <row r="327" ht="14.25" customHeight="1">
-      <c r="H327" s="12"/>
+      <c r="H327" s="15"/>
     </row>
     <row r="328" ht="14.25" customHeight="1">
-      <c r="H328" s="12"/>
+      <c r="H328" s="15"/>
     </row>
     <row r="329" ht="14.25" customHeight="1">
-      <c r="H329" s="12"/>
+      <c r="H329" s="15"/>
     </row>
     <row r="330" ht="14.25" customHeight="1">
-      <c r="H330" s="12"/>
+      <c r="H330" s="15"/>
     </row>
     <row r="331" ht="14.25" customHeight="1">
-      <c r="H331" s="12"/>
+      <c r="H331" s="15"/>
     </row>
     <row r="332" ht="14.25" customHeight="1">
-      <c r="H332" s="12"/>
+      <c r="H332" s="15"/>
     </row>
     <row r="333" ht="14.25" customHeight="1">
-      <c r="H333" s="12"/>
+      <c r="H333" s="15"/>
     </row>
     <row r="334" ht="14.25" customHeight="1">
-      <c r="H334" s="12"/>
+      <c r="H334" s="15"/>
     </row>
     <row r="335" ht="14.25" customHeight="1">
-      <c r="H335" s="12"/>
+      <c r="H335" s="15"/>
     </row>
     <row r="336" ht="14.25" customHeight="1">
-      <c r="H336" s="12"/>
+      <c r="H336" s="15"/>
     </row>
     <row r="337" ht="14.25" customHeight="1">
-      <c r="H337" s="12"/>
+      <c r="H337" s="15"/>
     </row>
     <row r="338" ht="14.25" customHeight="1">
-      <c r="H338" s="12"/>
+      <c r="H338" s="15"/>
     </row>
     <row r="339" ht="14.25" customHeight="1">
-      <c r="H339" s="12"/>
+      <c r="H339" s="15"/>
     </row>
     <row r="340" ht="14.25" customHeight="1">
-      <c r="H340" s="12"/>
+      <c r="H340" s="15"/>
     </row>
     <row r="341" ht="14.25" customHeight="1">
-      <c r="H341" s="12"/>
+      <c r="H341" s="15"/>
     </row>
     <row r="342" ht="14.25" customHeight="1">
-      <c r="H342" s="12"/>
+      <c r="H342" s="15"/>
     </row>
     <row r="343" ht="14.25" customHeight="1">
-      <c r="H343" s="12"/>
+      <c r="H343" s="15"/>
     </row>
     <row r="344" ht="14.25" customHeight="1">
-      <c r="H344" s="12"/>
+      <c r="H344" s="15"/>
     </row>
     <row r="345" ht="14.25" customHeight="1">
-      <c r="H345" s="12"/>
+      <c r="H345" s="15"/>
     </row>
     <row r="346" ht="14.25" customHeight="1">
-      <c r="H346" s="12"/>
+      <c r="H346" s="15"/>
     </row>
     <row r="347" ht="14.25" customHeight="1">
-      <c r="H347" s="12"/>
+      <c r="H347" s="15"/>
     </row>
     <row r="348" ht="14.25" customHeight="1">
-      <c r="H348" s="12"/>
+      <c r="H348" s="15"/>
     </row>
     <row r="349" ht="14.25" customHeight="1">
-      <c r="H349" s="12"/>
+      <c r="H349" s="15"/>
     </row>
     <row r="350" ht="14.25" customHeight="1">
-      <c r="H350" s="12"/>
+      <c r="H350" s="15"/>
     </row>
     <row r="351" ht="14.25" customHeight="1">
-      <c r="H351" s="12"/>
+      <c r="H351" s="15"/>
     </row>
     <row r="352" ht="14.25" customHeight="1">
-      <c r="H352" s="12"/>
+      <c r="H352" s="15"/>
     </row>
     <row r="353" ht="14.25" customHeight="1">
-      <c r="H353" s="12"/>
+      <c r="H353" s="15"/>
     </row>
     <row r="354" ht="14.25" customHeight="1">
-      <c r="H354" s="12"/>
+      <c r="H354" s="15"/>
     </row>
     <row r="355" ht="14.25" customHeight="1">
-      <c r="H355" s="12"/>
+      <c r="H355" s="15"/>
     </row>
     <row r="356" ht="14.25" customHeight="1">
-      <c r="H356" s="12"/>
+      <c r="H356" s="15"/>
     </row>
     <row r="357" ht="14.25" customHeight="1">
-      <c r="H357" s="12"/>
+      <c r="H357" s="15"/>
     </row>
     <row r="358" ht="14.25" customHeight="1">
-      <c r="H358" s="12"/>
+      <c r="H358" s="15"/>
     </row>
     <row r="359" ht="14.25" customHeight="1">
-      <c r="H359" s="12"/>
+      <c r="H359" s="15"/>
     </row>
     <row r="360" ht="14.25" customHeight="1">
-      <c r="H360" s="12"/>
+      <c r="H360" s="15"/>
     </row>
     <row r="361" ht="14.25" customHeight="1">
-      <c r="H361" s="12"/>
+      <c r="H361" s="15"/>
     </row>
     <row r="362" ht="14.25" customHeight="1">
-      <c r="H362" s="12"/>
+      <c r="H362" s="15"/>
     </row>
     <row r="363" ht="14.25" customHeight="1">
-      <c r="H363" s="12"/>
+      <c r="H363" s="15"/>
     </row>
     <row r="364" ht="14.25" customHeight="1">
-      <c r="H364" s="12"/>
+      <c r="H364" s="15"/>
     </row>
     <row r="365" ht="14.25" customHeight="1">
-      <c r="H365" s="12"/>
+      <c r="H365" s="15"/>
     </row>
     <row r="366" ht="14.25" customHeight="1">
-      <c r="H366" s="12"/>
+      <c r="H366" s="15"/>
     </row>
     <row r="367" ht="14.25" customHeight="1">
-      <c r="H367" s="12"/>
+      <c r="H367" s="15"/>
     </row>
     <row r="368" ht="14.25" customHeight="1">
-      <c r="H368" s="12"/>
+      <c r="H368" s="15"/>
     </row>
     <row r="369" ht="14.25" customHeight="1">
-      <c r="H369" s="12"/>
+      <c r="H369" s="15"/>
     </row>
     <row r="370" ht="14.25" customHeight="1">
-      <c r="H370" s="12"/>
+      <c r="H370" s="15"/>
     </row>
     <row r="371" ht="14.25" customHeight="1">
-      <c r="H371" s="12"/>
+      <c r="H371" s="15"/>
     </row>
     <row r="372" ht="14.25" customHeight="1">
-      <c r="H372" s="12"/>
+      <c r="H372" s="15"/>
     </row>
     <row r="373" ht="14.25" customHeight="1">
-      <c r="H373" s="12"/>
+      <c r="H373" s="15"/>
     </row>
     <row r="374" ht="14.25" customHeight="1">
-      <c r="H374" s="12"/>
+      <c r="H374" s="15"/>
     </row>
     <row r="375" ht="14.25" customHeight="1">
-      <c r="H375" s="12"/>
+      <c r="H375" s="15"/>
     </row>
     <row r="376" ht="14.25" customHeight="1">
-      <c r="H376" s="12"/>
+      <c r="H376" s="15"/>
     </row>
     <row r="377" ht="14.25" customHeight="1">
-      <c r="H377" s="12"/>
+      <c r="H377" s="15"/>
     </row>
     <row r="378" ht="14.25" customHeight="1">
-      <c r="H378" s="12"/>
+      <c r="H378" s="15"/>
     </row>
     <row r="379" ht="14.25" customHeight="1">
-      <c r="H379" s="12"/>
+      <c r="H379" s="15"/>
     </row>
     <row r="380" ht="14.25" customHeight="1">
-      <c r="H380" s="12"/>
+      <c r="H380" s="15"/>
     </row>
     <row r="381" ht="14.25" customHeight="1">
-      <c r="H381" s="12"/>
+      <c r="H381" s="15"/>
     </row>
     <row r="382" ht="14.25" customHeight="1">
-      <c r="H382" s="12"/>
+      <c r="H382" s="15"/>
     </row>
     <row r="383" ht="14.25" customHeight="1">
-      <c r="H383" s="12"/>
+      <c r="H383" s="15"/>
     </row>
     <row r="384" ht="14.25" customHeight="1">
-      <c r="H384" s="12"/>
+      <c r="H384" s="15"/>
     </row>
     <row r="385" ht="14.25" customHeight="1">
-      <c r="H385" s="12"/>
+      <c r="H385" s="15"/>
     </row>
     <row r="386" ht="14.25" customHeight="1">
-      <c r="H386" s="12"/>
+      <c r="H386" s="15"/>
     </row>
     <row r="387" ht="14.25" customHeight="1">
-      <c r="H387" s="12"/>
+      <c r="H387" s="15"/>
     </row>
     <row r="388" ht="14.25" customHeight="1">
-      <c r="H388" s="12"/>
+      <c r="H388" s="15"/>
     </row>
     <row r="389" ht="14.25" customHeight="1">
-      <c r="H389" s="12"/>
+      <c r="H389" s="15"/>
     </row>
     <row r="390" ht="14.25" customHeight="1">
-      <c r="H390" s="12"/>
+      <c r="H390" s="15"/>
     </row>
     <row r="391" ht="14.25" customHeight="1">
-      <c r="H391" s="12"/>
+      <c r="H391" s="15"/>
     </row>
     <row r="392" ht="14.25" customHeight="1">
-      <c r="H392" s="12"/>
+      <c r="H392" s="15"/>
     </row>
     <row r="393" ht="14.25" customHeight="1">
-      <c r="H393" s="12"/>
+      <c r="H393" s="15"/>
     </row>
     <row r="394" ht="14.25" customHeight="1">
-      <c r="H394" s="12"/>
+      <c r="H394" s="15"/>
     </row>
     <row r="395" ht="14.25" customHeight="1">
-      <c r="H395" s="12"/>
+      <c r="H395" s="15"/>
     </row>
     <row r="396" ht="14.25" customHeight="1">
-      <c r="H396" s="12"/>
+      <c r="H396" s="15"/>
     </row>
     <row r="397" ht="14.25" customHeight="1">
-      <c r="H397" s="12"/>
+      <c r="H397" s="15"/>
     </row>
     <row r="398" ht="14.25" customHeight="1">
-      <c r="H398" s="12"/>
+      <c r="H398" s="15"/>
     </row>
     <row r="399" ht="14.25" customHeight="1">
-      <c r="H399" s="12"/>
+      <c r="H399" s="15"/>
     </row>
     <row r="400" ht="14.25" customHeight="1">
-      <c r="H400" s="12"/>
+      <c r="H400" s="15"/>
     </row>
     <row r="401" ht="14.25" customHeight="1">
-      <c r="H401" s="12"/>
+      <c r="H401" s="15"/>
     </row>
     <row r="402" ht="14.25" customHeight="1">
-      <c r="H402" s="12"/>
+      <c r="H402" s="15"/>
     </row>
     <row r="403" ht="14.25" customHeight="1">
-      <c r="H403" s="12"/>
+      <c r="H403" s="15"/>
     </row>
     <row r="404" ht="14.25" customHeight="1">
-      <c r="H404" s="12"/>
+      <c r="H404" s="15"/>
     </row>
     <row r="405" ht="14.25" customHeight="1">
-      <c r="H405" s="12"/>
+      <c r="H405" s="15"/>
     </row>
     <row r="406" ht="14.25" customHeight="1">
-      <c r="H406" s="12"/>
+      <c r="H406" s="15"/>
     </row>
     <row r="407" ht="14.25" customHeight="1">
-      <c r="H407" s="12"/>
+      <c r="H407" s="15"/>
     </row>
     <row r="408" ht="14.25" customHeight="1">
-      <c r="H408" s="12"/>
+      <c r="H408" s="15"/>
     </row>
     <row r="409" ht="14.25" customHeight="1">
-      <c r="H409" s="12"/>
+      <c r="H409" s="15"/>
     </row>
     <row r="410" ht="14.25" customHeight="1">
-      <c r="H410" s="12"/>
+      <c r="H410" s="15"/>
     </row>
     <row r="411" ht="14.25" customHeight="1">
-      <c r="H411" s="12"/>
+      <c r="H411" s="15"/>
     </row>
     <row r="412" ht="14.25" customHeight="1">
-      <c r="H412" s="12"/>
+      <c r="H412" s="15"/>
     </row>
     <row r="413" ht="14.25" customHeight="1">
-      <c r="H413" s="12"/>
+      <c r="H413" s="15"/>
     </row>
     <row r="414" ht="14.25" customHeight="1">
-      <c r="H414" s="12"/>
+      <c r="H414" s="15"/>
     </row>
     <row r="415" ht="14.25" customHeight="1">
-      <c r="H415" s="12"/>
+      <c r="H415" s="15"/>
     </row>
     <row r="416" ht="14.25" customHeight="1">
-      <c r="H416" s="12"/>
+      <c r="H416" s="15"/>
     </row>
     <row r="417" ht="14.25" customHeight="1">
-      <c r="H417" s="12"/>
+      <c r="H417" s="15"/>
     </row>
     <row r="418" ht="14.25" customHeight="1">
-      <c r="H418" s="12"/>
+      <c r="H418" s="15"/>
     </row>
     <row r="419" ht="14.25" customHeight="1">
-      <c r="H419" s="12"/>
+      <c r="H419" s="15"/>
     </row>
     <row r="420" ht="14.25" customHeight="1">
-      <c r="H420" s="12"/>
+      <c r="H420" s="15"/>
     </row>
     <row r="421" ht="14.25" customHeight="1">
-      <c r="H421" s="12"/>
+      <c r="H421" s="15"/>
     </row>
     <row r="422" ht="14.25" customHeight="1">
-      <c r="H422" s="12"/>
+      <c r="H422" s="15"/>
     </row>
     <row r="423" ht="14.25" customHeight="1">
-      <c r="H423" s="12"/>
+      <c r="H423" s="15"/>
     </row>
     <row r="424" ht="14.25" customHeight="1">
-      <c r="H424" s="12"/>
+      <c r="H424" s="15"/>
     </row>
     <row r="425" ht="14.25" customHeight="1">
-      <c r="H425" s="12"/>
+      <c r="H425" s="15"/>
     </row>
     <row r="426" ht="14.25" customHeight="1">
-      <c r="H426" s="12"/>
+      <c r="H426" s="15"/>
     </row>
     <row r="427" ht="14.25" customHeight="1">
-      <c r="H427" s="12"/>
+      <c r="H427" s="15"/>
     </row>
     <row r="428" ht="14.25" customHeight="1">
-      <c r="H428" s="12"/>
+      <c r="H428" s="15"/>
     </row>
     <row r="429" ht="14.25" customHeight="1">
-      <c r="H429" s="12"/>
+      <c r="H429" s="15"/>
     </row>
     <row r="430" ht="14.25" customHeight="1">
-      <c r="H430" s="12"/>
+      <c r="H430" s="15"/>
     </row>
     <row r="431" ht="14.25" customHeight="1">
-      <c r="H431" s="12"/>
+      <c r="H431" s="15"/>
     </row>
     <row r="432" ht="14.25" customHeight="1">
-      <c r="H432" s="12"/>
+      <c r="H432" s="15"/>
     </row>
     <row r="433" ht="14.25" customHeight="1">
-      <c r="H433" s="12"/>
+      <c r="H433" s="15"/>
     </row>
     <row r="434" ht="14.25" customHeight="1">
-      <c r="H434" s="12"/>
+      <c r="H434" s="15"/>
     </row>
     <row r="435" ht="14.25" customHeight="1">
-      <c r="H435" s="12"/>
+      <c r="H435" s="15"/>
     </row>
     <row r="436" ht="14.25" customHeight="1">
-      <c r="H436" s="12"/>
+      <c r="H436" s="15"/>
     </row>
     <row r="437" ht="14.25" customHeight="1">
-      <c r="H437" s="12"/>
+      <c r="H437" s="15"/>
     </row>
     <row r="438" ht="14.25" customHeight="1">
-      <c r="H438" s="12"/>
+      <c r="H438" s="15"/>
     </row>
     <row r="439" ht="14.25" customHeight="1">
-      <c r="H439" s="12"/>
+      <c r="H439" s="15"/>
     </row>
     <row r="440" ht="14.25" customHeight="1">
-      <c r="H440" s="12"/>
+      <c r="H440" s="15"/>
     </row>
     <row r="441" ht="14.25" customHeight="1">
-      <c r="H441" s="12"/>
+      <c r="H441" s="15"/>
     </row>
     <row r="442" ht="14.25" customHeight="1">
-      <c r="H442" s="12"/>
+      <c r="H442" s="15"/>
     </row>
     <row r="443" ht="14.25" customHeight="1">
-      <c r="H443" s="12"/>
+      <c r="H443" s="15"/>
     </row>
     <row r="444" ht="14.25" customHeight="1">
-      <c r="H444" s="12"/>
+      <c r="H444" s="15"/>
     </row>
     <row r="445" ht="14.25" customHeight="1">
-      <c r="H445" s="12"/>
+      <c r="H445" s="15"/>
     </row>
     <row r="446" ht="14.25" customHeight="1">
-      <c r="H446" s="12"/>
+      <c r="H446" s="15"/>
     </row>
     <row r="447" ht="14.25" customHeight="1">
-      <c r="H447" s="12"/>
+      <c r="H447" s="15"/>
     </row>
     <row r="448" ht="14.25" customHeight="1">
-      <c r="H448" s="12"/>
+      <c r="H448" s="15"/>
     </row>
     <row r="449" ht="14.25" customHeight="1">
-      <c r="H449" s="12"/>
+      <c r="H449" s="15"/>
     </row>
     <row r="450" ht="14.25" customHeight="1">
-      <c r="H450" s="12"/>
+      <c r="H450" s="15"/>
     </row>
     <row r="451" ht="14.25" customHeight="1">
-      <c r="H451" s="12"/>
+      <c r="H451" s="15"/>
     </row>
     <row r="452" ht="14.25" customHeight="1">
-      <c r="H452" s="12"/>
+      <c r="H452" s="15"/>
     </row>
     <row r="453" ht="14.25" customHeight="1">
-      <c r="H453" s="12"/>
+      <c r="H453" s="15"/>
     </row>
     <row r="454" ht="14.25" customHeight="1">
-      <c r="H454" s="12"/>
+      <c r="H454" s="15"/>
     </row>
     <row r="455" ht="14.25" customHeight="1">
-      <c r="H455" s="12"/>
+      <c r="H455" s="15"/>
     </row>
     <row r="456" ht="14.25" customHeight="1">
-      <c r="H456" s="12"/>
+      <c r="H456" s="15"/>
     </row>
     <row r="457" ht="14.25" customHeight="1">
-      <c r="H457" s="12"/>
+      <c r="H457" s="15"/>
     </row>
     <row r="458" ht="14.25" customHeight="1">
-      <c r="H458" s="12"/>
+      <c r="H458" s="15"/>
     </row>
     <row r="459" ht="14.25" customHeight="1">
-      <c r="H459" s="12"/>
+      <c r="H459" s="15"/>
     </row>
     <row r="460" ht="14.25" customHeight="1">
-      <c r="H460" s="12"/>
+      <c r="H460" s="15"/>
     </row>
     <row r="461" ht="14.25" customHeight="1">
-      <c r="H461" s="12"/>
+      <c r="H461" s="15"/>
     </row>
     <row r="462" ht="14.25" customHeight="1">
-      <c r="H462" s="12"/>
+      <c r="H462" s="15"/>
     </row>
     <row r="463" ht="14.25" customHeight="1">
-      <c r="H463" s="12"/>
+      <c r="H463" s="15"/>
     </row>
     <row r="464" ht="14.25" customHeight="1">
-      <c r="H464" s="12"/>
+      <c r="H464" s="15"/>
     </row>
     <row r="465" ht="14.25" customHeight="1">
-      <c r="H465" s="12"/>
+      <c r="H465" s="15"/>
     </row>
     <row r="466" ht="14.25" customHeight="1">
-      <c r="H466" s="12"/>
+      <c r="H466" s="15"/>
     </row>
     <row r="467" ht="14.25" customHeight="1">
-      <c r="H467" s="12"/>
+      <c r="H467" s="15"/>
     </row>
     <row r="468" ht="14.25" customHeight="1">
-      <c r="H468" s="12"/>
+      <c r="H468" s="15"/>
     </row>
     <row r="469" ht="14.25" customHeight="1">
-      <c r="H469" s="12"/>
+      <c r="H469" s="15"/>
     </row>
     <row r="470" ht="14.25" customHeight="1">
-      <c r="H470" s="12"/>
+      <c r="H470" s="15"/>
     </row>
     <row r="471" ht="14.25" customHeight="1">
-      <c r="H471" s="12"/>
+      <c r="H471" s="15"/>
     </row>
     <row r="472" ht="14.25" customHeight="1">
-      <c r="H472" s="12"/>
+      <c r="H472" s="15"/>
     </row>
     <row r="473" ht="14.25" customHeight="1">
-      <c r="H473" s="12"/>
+      <c r="H473" s="15"/>
     </row>
     <row r="474" ht="14.25" customHeight="1">
-      <c r="H474" s="12"/>
+      <c r="H474" s="15"/>
     </row>
     <row r="475" ht="14.25" customHeight="1">
-      <c r="H475" s="12"/>
+      <c r="H475" s="15"/>
     </row>
     <row r="476" ht="14.25" customHeight="1">
-      <c r="H476" s="12"/>
+      <c r="H476" s="15"/>
     </row>
     <row r="477" ht="14.25" customHeight="1">
-      <c r="H477" s="12"/>
+      <c r="H477" s="15"/>
     </row>
     <row r="478" ht="14.25" customHeight="1">
-      <c r="H478" s="12"/>
+      <c r="H478" s="15"/>
     </row>
     <row r="479" ht="14.25" customHeight="1">
-      <c r="H479" s="12"/>
+      <c r="H479" s="15"/>
     </row>
     <row r="480" ht="14.25" customHeight="1">
-      <c r="H480" s="12"/>
+      <c r="H480" s="15"/>
     </row>
     <row r="481" ht="14.25" customHeight="1">
-      <c r="H481" s="12"/>
+      <c r="H481" s="15"/>
     </row>
     <row r="482" ht="14.25" customHeight="1">
-      <c r="H482" s="12"/>
+      <c r="H482" s="15"/>
     </row>
     <row r="483" ht="14.25" customHeight="1">
-      <c r="H483" s="12"/>
+      <c r="H483" s="15"/>
     </row>
     <row r="484" ht="14.25" customHeight="1">
-      <c r="H484" s="12"/>
+      <c r="H484" s="15"/>
     </row>
     <row r="485" ht="14.25" customHeight="1">
-      <c r="H485" s="12"/>
+      <c r="H485" s="15"/>
     </row>
     <row r="486" ht="14.25" customHeight="1">
-      <c r="H486" s="12"/>
+      <c r="H486" s="15"/>
     </row>
     <row r="487" ht="14.25" customHeight="1">
-      <c r="H487" s="12"/>
+      <c r="H487" s="15"/>
     </row>
     <row r="488" ht="14.25" customHeight="1">
-      <c r="H488" s="12"/>
+      <c r="H488" s="15"/>
     </row>
     <row r="489" ht="14.25" customHeight="1">
-      <c r="H489" s="12"/>
+      <c r="H489" s="15"/>
     </row>
     <row r="490" ht="14.25" customHeight="1">
-      <c r="H490" s="12"/>
+      <c r="H490" s="15"/>
     </row>
     <row r="491" ht="14.25" customHeight="1">
-      <c r="H491" s="12"/>
+      <c r="H491" s="15"/>
     </row>
     <row r="492" ht="14.25" customHeight="1">
-      <c r="H492" s="12"/>
+      <c r="H492" s="15"/>
     </row>
     <row r="493" ht="14.25" customHeight="1">
-      <c r="H493" s="12"/>
+      <c r="H493" s="15"/>
     </row>
     <row r="494" ht="14.25" customHeight="1">
-      <c r="H494" s="12"/>
+      <c r="H494" s="15"/>
     </row>
     <row r="495" ht="14.25" customHeight="1">
-      <c r="H495" s="12"/>
+      <c r="H495" s="15"/>
     </row>
     <row r="496" ht="14.25" customHeight="1">
-      <c r="H496" s="12"/>
+      <c r="H496" s="15"/>
     </row>
     <row r="497" ht="14.25" customHeight="1">
-      <c r="H497" s="12"/>
+      <c r="H497" s="15"/>
     </row>
     <row r="498" ht="14.25" customHeight="1">
-      <c r="H498" s="12"/>
+      <c r="H498" s="15"/>
     </row>
     <row r="499" ht="14.25" customHeight="1">
-      <c r="H499" s="12"/>
+      <c r="H499" s="15"/>
     </row>
     <row r="500" ht="14.25" customHeight="1">
-      <c r="H500" s="12"/>
+      <c r="H500" s="15"/>
     </row>
     <row r="501" ht="14.25" customHeight="1">
-      <c r="H501" s="12"/>
+      <c r="H501" s="15"/>
     </row>
     <row r="502" ht="14.25" customHeight="1">
-      <c r="H502" s="12"/>
+      <c r="H502" s="15"/>
     </row>
     <row r="503" ht="14.25" customHeight="1">
-      <c r="H503" s="12"/>
+      <c r="H503" s="15"/>
     </row>
     <row r="504" ht="14.25" customHeight="1">
-      <c r="H504" s="12"/>
+      <c r="H504" s="15"/>
     </row>
     <row r="505" ht="14.25" customHeight="1">
-      <c r="H505" s="12"/>
+      <c r="H505" s="15"/>
     </row>
     <row r="506" ht="14.25" customHeight="1">
-      <c r="H506" s="12"/>
+      <c r="H506" s="15"/>
     </row>
     <row r="507" ht="14.25" customHeight="1">
-      <c r="H507" s="12"/>
+      <c r="H507" s="15"/>
     </row>
     <row r="508" ht="14.25" customHeight="1">
-      <c r="H508" s="12"/>
+      <c r="H508" s="15"/>
     </row>
     <row r="509" ht="14.25" customHeight="1">
-      <c r="H509" s="12"/>
+      <c r="H509" s="15"/>
     </row>
     <row r="510" ht="14.25" customHeight="1">
-      <c r="H510" s="12"/>
+      <c r="H510" s="15"/>
     </row>
     <row r="511" ht="14.25" customHeight="1">
-      <c r="H511" s="12"/>
+      <c r="H511" s="15"/>
     </row>
     <row r="512" ht="14.25" customHeight="1">
-      <c r="H512" s="12"/>
+      <c r="H512" s="15"/>
     </row>
     <row r="513" ht="14.25" customHeight="1">
-      <c r="H513" s="12"/>
+      <c r="H513" s="15"/>
     </row>
     <row r="514" ht="14.25" customHeight="1">
-      <c r="H514" s="12"/>
+      <c r="H514" s="15"/>
     </row>
     <row r="515" ht="14.25" customHeight="1">
-      <c r="H515" s="12"/>
+      <c r="H515" s="15"/>
     </row>
     <row r="516" ht="14.25" customHeight="1">
-      <c r="H516" s="12"/>
+      <c r="H516" s="15"/>
     </row>
     <row r="517" ht="14.25" customHeight="1">
-      <c r="H517" s="12"/>
+      <c r="H517" s="15"/>
     </row>
     <row r="518" ht="14.25" customHeight="1">
-      <c r="H518" s="12"/>
+      <c r="H518" s="15"/>
     </row>
     <row r="519" ht="14.25" customHeight="1">
-      <c r="H519" s="12"/>
+      <c r="H519" s="15"/>
     </row>
     <row r="520" ht="14.25" customHeight="1">
-      <c r="H520" s="12"/>
+      <c r="H520" s="15"/>
     </row>
     <row r="521" ht="14.25" customHeight="1">
-      <c r="H521" s="12"/>
+      <c r="H521" s="15"/>
     </row>
     <row r="522" ht="14.25" customHeight="1">
-      <c r="H522" s="12"/>
+      <c r="H522" s="15"/>
     </row>
     <row r="523" ht="14.25" customHeight="1">
-      <c r="H523" s="12"/>
+      <c r="H523" s="15"/>
     </row>
     <row r="524" ht="14.25" customHeight="1">
-      <c r="H524" s="12"/>
+      <c r="H524" s="15"/>
     </row>
     <row r="525" ht="14.25" customHeight="1">
-      <c r="H525" s="12"/>
+      <c r="H525" s="15"/>
     </row>
     <row r="526" ht="14.25" customHeight="1">
-      <c r="H526" s="12"/>
+      <c r="H526" s="15"/>
     </row>
     <row r="527" ht="14.25" customHeight="1">
-      <c r="H527" s="12"/>
+      <c r="H527" s="15"/>
     </row>
     <row r="528" ht="14.25" customHeight="1">
-      <c r="H528" s="12"/>
+      <c r="H528" s="15"/>
     </row>
     <row r="529" ht="14.25" customHeight="1">
-      <c r="H529" s="12"/>
+      <c r="H529" s="15"/>
     </row>
     <row r="530" ht="14.25" customHeight="1">
-      <c r="H530" s="12"/>
+      <c r="H530" s="15"/>
     </row>
     <row r="531" ht="14.25" customHeight="1">
-      <c r="H531" s="12"/>
+      <c r="H531" s="15"/>
     </row>
     <row r="532" ht="14.25" customHeight="1">
-      <c r="H532" s="12"/>
+      <c r="H532" s="15"/>
     </row>
     <row r="533" ht="14.25" customHeight="1">
-      <c r="H533" s="12"/>
+      <c r="H533" s="15"/>
     </row>
     <row r="534" ht="14.25" customHeight="1">
-      <c r="H534" s="12"/>
+      <c r="H534" s="15"/>
     </row>
     <row r="535" ht="14.25" customHeight="1">
-      <c r="H535" s="12"/>
+      <c r="H535" s="15"/>
     </row>
     <row r="536" ht="14.25" customHeight="1">
-      <c r="H536" s="12"/>
+      <c r="H536" s="15"/>
     </row>
     <row r="537" ht="14.25" customHeight="1">
-      <c r="H537" s="12"/>
+      <c r="H537" s="15"/>
     </row>
     <row r="538" ht="14.25" customHeight="1">
-      <c r="H538" s="12"/>
+      <c r="H538" s="15"/>
     </row>
     <row r="539" ht="14.25" customHeight="1">
-      <c r="H539" s="12"/>
+      <c r="H539" s="15"/>
     </row>
     <row r="540" ht="14.25" customHeight="1">
-      <c r="H540" s="12"/>
+      <c r="H540" s="15"/>
     </row>
     <row r="541" ht="14.25" customHeight="1">
-      <c r="H541" s="12"/>
+      <c r="H541" s="15"/>
     </row>
     <row r="542" ht="14.25" customHeight="1">
-      <c r="H542" s="12"/>
+      <c r="H542" s="15"/>
     </row>
     <row r="543" ht="14.25" customHeight="1">
-      <c r="H543" s="12"/>
+      <c r="H543" s="15"/>
     </row>
     <row r="544" ht="14.25" customHeight="1">
-      <c r="H544" s="12"/>
+      <c r="H544" s="15"/>
     </row>
     <row r="545" ht="14.25" customHeight="1">
-      <c r="H545" s="12"/>
+      <c r="H545" s="15"/>
     </row>
     <row r="546" ht="14.25" customHeight="1">
-      <c r="H546" s="12"/>
+      <c r="H546" s="15"/>
     </row>
     <row r="547" ht="14.25" customHeight="1">
-      <c r="H547" s="12"/>
+      <c r="H547" s="15"/>
     </row>
     <row r="548" ht="14.25" customHeight="1">
-      <c r="H548" s="12"/>
+      <c r="H548" s="15"/>
     </row>
     <row r="549" ht="14.25" customHeight="1">
-      <c r="H549" s="12"/>
+      <c r="H549" s="15"/>
     </row>
     <row r="550" ht="14.25" customHeight="1">
-      <c r="H550" s="12"/>
+      <c r="H550" s="15"/>
     </row>
     <row r="551" ht="14.25" customHeight="1">
-      <c r="H551" s="12"/>
+      <c r="H551" s="15"/>
     </row>
     <row r="552" ht="14.25" customHeight="1">
-      <c r="H552" s="12"/>
+      <c r="H552" s="15"/>
     </row>
     <row r="553" ht="14.25" customHeight="1">
-      <c r="H553" s="12"/>
+      <c r="H553" s="15"/>
     </row>
     <row r="554" ht="14.25" customHeight="1">
-      <c r="H554" s="12"/>
+      <c r="H554" s="15"/>
     </row>
     <row r="555" ht="14.25" customHeight="1">
-      <c r="H555" s="12"/>
+      <c r="H555" s="15"/>
     </row>
     <row r="556" ht="14.25" customHeight="1">
-      <c r="H556" s="12"/>
+      <c r="H556" s="15"/>
     </row>
     <row r="557" ht="14.25" customHeight="1">
-      <c r="H557" s="12"/>
+      <c r="H557" s="15"/>
     </row>
     <row r="558" ht="14.25" customHeight="1">
-      <c r="H558" s="12"/>
+      <c r="H558" s="15"/>
     </row>
     <row r="559" ht="14.25" customHeight="1">
-      <c r="H559" s="12"/>
+      <c r="H559" s="15"/>
     </row>
     <row r="560" ht="14.25" customHeight="1">
-      <c r="H560" s="12"/>
+      <c r="H560" s="15"/>
     </row>
     <row r="561" ht="14.25" customHeight="1">
-      <c r="H561" s="12"/>
+      <c r="H561" s="15"/>
     </row>
     <row r="562" ht="14.25" customHeight="1">
-      <c r="H562" s="12"/>
+      <c r="H562" s="15"/>
     </row>
     <row r="563" ht="14.25" customHeight="1">
-      <c r="H563" s="12"/>
+      <c r="H563" s="15"/>
     </row>
     <row r="564" ht="14.25" customHeight="1">
-      <c r="H564" s="12"/>
+      <c r="H564" s="15"/>
     </row>
     <row r="565" ht="14.25" customHeight="1">
-      <c r="H565" s="12"/>
+      <c r="H565" s="15"/>
     </row>
     <row r="566" ht="14.25" customHeight="1">
-      <c r="H566" s="12"/>
+      <c r="H566" s="15"/>
     </row>
     <row r="567" ht="14.25" customHeight="1">
-      <c r="H567" s="12"/>
+      <c r="H567" s="15"/>
     </row>
     <row r="568" ht="14.25" customHeight="1">
-      <c r="H568" s="12"/>
+      <c r="H568" s="15"/>
     </row>
     <row r="569" ht="14.25" customHeight="1">
-      <c r="H569" s="12"/>
+      <c r="H569" s="15"/>
     </row>
     <row r="570" ht="14.25" customHeight="1">
-      <c r="H570" s="12"/>
+      <c r="H570" s="15"/>
     </row>
     <row r="571" ht="14.25" customHeight="1">
-      <c r="H571" s="12"/>
+      <c r="H571" s="15"/>
     </row>
     <row r="572" ht="14.25" customHeight="1">
-      <c r="H572" s="12"/>
+      <c r="H572" s="15"/>
     </row>
     <row r="573" ht="14.25" customHeight="1">
-      <c r="H573" s="12"/>
+      <c r="H573" s="15"/>
     </row>
     <row r="574" ht="14.25" customHeight="1">
-      <c r="H574" s="12"/>
+      <c r="H574" s="15"/>
     </row>
     <row r="575" ht="14.25" customHeight="1">
-      <c r="H575" s="12"/>
+      <c r="H575" s="15"/>
     </row>
     <row r="576" ht="14.25" customHeight="1">
-      <c r="H576" s="12"/>
+      <c r="H576" s="15"/>
     </row>
     <row r="577" ht="14.25" customHeight="1">
-      <c r="H577" s="12"/>
+      <c r="H577" s="15"/>
     </row>
     <row r="578" ht="14.25" customHeight="1">
-      <c r="H578" s="12"/>
+      <c r="H578" s="15"/>
     </row>
     <row r="579" ht="14.25" customHeight="1">
-      <c r="H579" s="12"/>
+      <c r="H579" s="15"/>
     </row>
     <row r="580" ht="14.25" customHeight="1">
-      <c r="H580" s="12"/>
+      <c r="H580" s="15"/>
     </row>
     <row r="581" ht="14.25" customHeight="1">
-      <c r="H581" s="12"/>
+      <c r="H581" s="15"/>
     </row>
     <row r="582" ht="14.25" customHeight="1">
-      <c r="H582" s="12"/>
+      <c r="H582" s="15"/>
     </row>
     <row r="583" ht="14.25" customHeight="1">
-      <c r="H583" s="12"/>
+      <c r="H583" s="15"/>
     </row>
     <row r="584" ht="14.25" customHeight="1">
-      <c r="H584" s="12"/>
+      <c r="H584" s="15"/>
     </row>
     <row r="585" ht="14.25" customHeight="1">
-      <c r="H585" s="12"/>
+      <c r="H585" s="15"/>
     </row>
     <row r="586" ht="14.25" customHeight="1">
-      <c r="H586" s="12"/>
+      <c r="H586" s="15"/>
     </row>
     <row r="587" ht="14.25" customHeight="1">
-      <c r="H587" s="12"/>
+      <c r="H587" s="15"/>
     </row>
     <row r="588" ht="14.25" customHeight="1">
-      <c r="H588" s="12"/>
+      <c r="H588" s="15"/>
     </row>
     <row r="589" ht="14.25" customHeight="1">
-      <c r="H589" s="12"/>
+      <c r="H589" s="15"/>
     </row>
     <row r="590" ht="14.25" customHeight="1">
-      <c r="H590" s="12"/>
+      <c r="H590" s="15"/>
     </row>
     <row r="591" ht="14.25" customHeight="1">
-      <c r="H591" s="12"/>
+      <c r="H591" s="15"/>
     </row>
     <row r="592" ht="14.25" customHeight="1">
-      <c r="H592" s="12"/>
+      <c r="H592" s="15"/>
     </row>
     <row r="593" ht="14.25" customHeight="1">
-      <c r="H593" s="12"/>
+      <c r="H593" s="15"/>
     </row>
     <row r="594" ht="14.25" customHeight="1">
-      <c r="H594" s="12"/>
+      <c r="H594" s="15"/>
     </row>
     <row r="595" ht="14.25" customHeight="1">
-      <c r="H595" s="12"/>
+      <c r="H595" s="15"/>
     </row>
     <row r="596" ht="14.25" customHeight="1">
-      <c r="H596" s="12"/>
+      <c r="H596" s="15"/>
     </row>
     <row r="597" ht="14.25" customHeight="1">
-      <c r="H597" s="12"/>
+      <c r="H597" s="15"/>
     </row>
     <row r="598" ht="14.25" customHeight="1">
-      <c r="H598" s="12"/>
+      <c r="H598" s="15"/>
     </row>
     <row r="599" ht="14.25" customHeight="1">
-      <c r="H599" s="12"/>
+      <c r="H599" s="15"/>
     </row>
     <row r="600" ht="14.25" customHeight="1">
-      <c r="H600" s="12"/>
+      <c r="H600" s="15"/>
     </row>
     <row r="601" ht="14.25" customHeight="1">
-      <c r="H601" s="12"/>
+      <c r="H601" s="15"/>
     </row>
     <row r="602" ht="14.25" customHeight="1">
-      <c r="H602" s="12"/>
+      <c r="H602" s="15"/>
     </row>
     <row r="603" ht="14.25" customHeight="1">
-      <c r="H603" s="12"/>
+      <c r="H603" s="15"/>
     </row>
     <row r="604" ht="14.25" customHeight="1">
-      <c r="H604" s="12"/>
+      <c r="H604" s="15"/>
     </row>
     <row r="605" ht="14.25" customHeight="1">
-      <c r="H605" s="12"/>
+      <c r="H605" s="15"/>
     </row>
     <row r="606" ht="14.25" customHeight="1">
-      <c r="H606" s="12"/>
+      <c r="H606" s="15"/>
     </row>
     <row r="607" ht="14.25" customHeight="1">
-      <c r="H607" s="12"/>
+      <c r="H607" s="15"/>
     </row>
     <row r="608" ht="14.25" customHeight="1">
-      <c r="H608" s="12"/>
+      <c r="H608" s="15"/>
     </row>
     <row r="609" ht="14.25" customHeight="1">
-      <c r="H609" s="12"/>
+      <c r="H609" s="15"/>
     </row>
     <row r="610" ht="14.25" customHeight="1">
-      <c r="H610" s="12"/>
+      <c r="H610" s="15"/>
     </row>
     <row r="611" ht="14.25" customHeight="1">
-      <c r="H611" s="12"/>
+      <c r="H611" s="15"/>
     </row>
     <row r="612" ht="14.25" customHeight="1">
-      <c r="H612" s="12"/>
+      <c r="H612" s="15"/>
     </row>
     <row r="613" ht="14.25" customHeight="1">
-      <c r="H613" s="12"/>
+      <c r="H613" s="15"/>
     </row>
     <row r="614" ht="14.25" customHeight="1">
-      <c r="H614" s="12"/>
+      <c r="H614" s="15"/>
     </row>
     <row r="615" ht="14.25" customHeight="1">
-      <c r="H615" s="12"/>
+      <c r="H615" s="15"/>
     </row>
     <row r="616" ht="14.25" customHeight="1">
-      <c r="H616" s="12"/>
+      <c r="H616" s="15"/>
     </row>
     <row r="617" ht="14.25" customHeight="1">
-      <c r="H617" s="12"/>
+      <c r="H617" s="15"/>
     </row>
     <row r="618" ht="14.25" customHeight="1">
-      <c r="H618" s="12"/>
+      <c r="H618" s="15"/>
     </row>
     <row r="619" ht="14.25" customHeight="1">
-      <c r="H619" s="12"/>
+      <c r="H619" s="15"/>
     </row>
     <row r="620" ht="14.25" customHeight="1">
-      <c r="H620" s="12"/>
+      <c r="H620" s="15"/>
     </row>
     <row r="621" ht="14.25" customHeight="1">
-      <c r="H621" s="12"/>
+      <c r="H621" s="15"/>
     </row>
     <row r="622" ht="14.25" customHeight="1">
-      <c r="H622" s="12"/>
+      <c r="H622" s="15"/>
     </row>
     <row r="623" ht="14.25" customHeight="1">
-      <c r="H623" s="12"/>
+      <c r="H623" s="15"/>
     </row>
     <row r="624" ht="14.25" customHeight="1">
-      <c r="H624" s="12"/>
+      <c r="H624" s="15"/>
     </row>
     <row r="625" ht="14.25" customHeight="1">
-      <c r="H625" s="12"/>
+      <c r="H625" s="15"/>
     </row>
     <row r="626" ht="14.25" customHeight="1">
-      <c r="H626" s="12"/>
+      <c r="H626" s="15"/>
     </row>
     <row r="627" ht="14.25" customHeight="1">
-      <c r="H627" s="12"/>
+      <c r="H627" s="15"/>
     </row>
     <row r="628" ht="14.25" customHeight="1">
-      <c r="H628" s="12"/>
+      <c r="H628" s="15"/>
     </row>
     <row r="629" ht="14.25" customHeight="1">
-      <c r="H629" s="12"/>
+      <c r="H629" s="15"/>
     </row>
     <row r="630" ht="14.25" customHeight="1">
-      <c r="H630" s="12"/>
+      <c r="H630" s="15"/>
     </row>
     <row r="631" ht="14.25" customHeight="1">
-      <c r="H631" s="12"/>
+      <c r="H631" s="15"/>
     </row>
     <row r="632" ht="14.25" customHeight="1">
-      <c r="H632" s="12"/>
+      <c r="H632" s="15"/>
     </row>
     <row r="633" ht="14.25" customHeight="1">
-      <c r="H633" s="12"/>
+      <c r="H633" s="15"/>
     </row>
     <row r="634" ht="14.25" customHeight="1">
-      <c r="H634" s="12"/>
+      <c r="H634" s="15"/>
     </row>
     <row r="635" ht="14.25" customHeight="1">
-      <c r="H635" s="12"/>
+      <c r="H635" s="15"/>
     </row>
     <row r="636" ht="14.25" customHeight="1">
-      <c r="H636" s="12"/>
+      <c r="H636" s="15"/>
     </row>
     <row r="637" ht="14.25" customHeight="1">
-      <c r="H637" s="12"/>
+      <c r="H637" s="15"/>
     </row>
     <row r="638" ht="14.25" customHeight="1">
-      <c r="H638" s="12"/>
+      <c r="H638" s="15"/>
     </row>
     <row r="639" ht="14.25" customHeight="1">
-      <c r="H639" s="12"/>
+      <c r="H639" s="15"/>
     </row>
     <row r="640" ht="14.25" customHeight="1">
-      <c r="H640" s="12"/>
+      <c r="H640" s="15"/>
     </row>
     <row r="641" ht="14.25" customHeight="1">
-      <c r="H641" s="12"/>
+      <c r="H641" s="15"/>
     </row>
     <row r="642" ht="14.25" customHeight="1">
-      <c r="H642" s="12"/>
+      <c r="H642" s="15"/>
     </row>
     <row r="643" ht="14.25" customHeight="1">
-      <c r="H643" s="12"/>
+      <c r="H643" s="15"/>
     </row>
     <row r="644" ht="14.25" customHeight="1">
-      <c r="H644" s="12"/>
+      <c r="H644" s="15"/>
     </row>
     <row r="645" ht="14.25" customHeight="1">
-      <c r="H645" s="12"/>
+      <c r="H645" s="15"/>
     </row>
     <row r="646" ht="14.25" customHeight="1">
-      <c r="H646" s="12"/>
+      <c r="H646" s="15"/>
     </row>
     <row r="647" ht="14.25" customHeight="1">
-      <c r="H647" s="12"/>
+      <c r="H647" s="15"/>
     </row>
     <row r="648" ht="14.25" customHeight="1">
-      <c r="H648" s="12"/>
+      <c r="H648" s="15"/>
     </row>
     <row r="649" ht="14.25" customHeight="1">
-      <c r="H649" s="12"/>
+      <c r="H649" s="15"/>
     </row>
     <row r="650" ht="14.25" customHeight="1">
-      <c r="H650" s="12"/>
+      <c r="H650" s="15"/>
     </row>
     <row r="651" ht="14.25" customHeight="1">
-      <c r="H651" s="12"/>
+      <c r="H651" s="15"/>
     </row>
     <row r="652" ht="14.25" customHeight="1">
-      <c r="H652" s="12"/>
+      <c r="H652" s="15"/>
     </row>
     <row r="653" ht="14.25" customHeight="1">
-      <c r="H653" s="12"/>
+      <c r="H653" s="15"/>
     </row>
     <row r="654" ht="14.25" customHeight="1">
-      <c r="H654" s="12"/>
+      <c r="H654" s="15"/>
     </row>
     <row r="655" ht="14.25" customHeight="1">
-      <c r="H655" s="12"/>
+      <c r="H655" s="15"/>
     </row>
     <row r="656" ht="14.25" customHeight="1">
-      <c r="H656" s="12"/>
+      <c r="H656" s="15"/>
     </row>
     <row r="657" ht="14.25" customHeight="1">
-      <c r="H657" s="12"/>
+      <c r="H657" s="15"/>
     </row>
     <row r="658" ht="14.25" customHeight="1">
-      <c r="H658" s="12"/>
+      <c r="H658" s="15"/>
     </row>
     <row r="659" ht="14.25" customHeight="1">
-      <c r="H659" s="12"/>
+      <c r="H659" s="15"/>
     </row>
     <row r="660" ht="14.25" customHeight="1">
-      <c r="H660" s="12"/>
+      <c r="H660" s="15"/>
     </row>
     <row r="661" ht="14.25" customHeight="1">
-      <c r="H661" s="12"/>
+      <c r="H661" s="15"/>
     </row>
     <row r="662" ht="14.25" customHeight="1">
-      <c r="H662" s="12"/>
+      <c r="H662" s="15"/>
     </row>
     <row r="663" ht="14.25" customHeight="1">
-      <c r="H663" s="12"/>
+      <c r="H663" s="15"/>
     </row>
     <row r="664" ht="14.25" customHeight="1">
-      <c r="H664" s="12"/>
+      <c r="H664" s="15"/>
     </row>
     <row r="665" ht="14.25" customHeight="1">
-      <c r="H665" s="12"/>
+      <c r="H665" s="15"/>
     </row>
     <row r="666" ht="14.25" customHeight="1">
-      <c r="H666" s="12"/>
+      <c r="H666" s="15"/>
     </row>
     <row r="667" ht="14.25" customHeight="1">
-      <c r="H667" s="12"/>
+      <c r="H667" s="15"/>
     </row>
     <row r="668" ht="14.25" customHeight="1">
-      <c r="H668" s="12"/>
+      <c r="H668" s="15"/>
     </row>
     <row r="669" ht="14.25" customHeight="1">
-      <c r="H669" s="12"/>
+      <c r="H669" s="15"/>
     </row>
     <row r="670" ht="14.25" customHeight="1">
-      <c r="H670" s="12"/>
+      <c r="H670" s="15"/>
     </row>
     <row r="671" ht="14.25" customHeight="1">
-      <c r="H671" s="12"/>
+      <c r="H671" s="15"/>
     </row>
     <row r="672" ht="14.25" customHeight="1">
-      <c r="H672" s="12"/>
+      <c r="H672" s="15"/>
     </row>
     <row r="673" ht="14.25" customHeight="1">
-      <c r="H673" s="12"/>
+      <c r="H673" s="15"/>
     </row>
     <row r="674" ht="14.25" customHeight="1">
-      <c r="H674" s="12"/>
+      <c r="H674" s="15"/>
     </row>
     <row r="675" ht="14.25" customHeight="1">
-      <c r="H675" s="12"/>
+      <c r="H675" s="15"/>
     </row>
     <row r="676" ht="14.25" customHeight="1">
-      <c r="H676" s="12"/>
+      <c r="H676" s="15"/>
     </row>
     <row r="677" ht="14.25" customHeight="1">
-      <c r="H677" s="12"/>
+      <c r="H677" s="15"/>
     </row>
     <row r="678" ht="14.25" customHeight="1">
-      <c r="H678" s="12"/>
+      <c r="H678" s="15"/>
     </row>
     <row r="679" ht="14.25" customHeight="1">
-      <c r="H679" s="12"/>
+      <c r="H679" s="15"/>
     </row>
     <row r="680" ht="14.25" customHeight="1">
-      <c r="H680" s="12"/>
+      <c r="H680" s="15"/>
     </row>
     <row r="681" ht="14.25" customHeight="1">
-      <c r="H681" s="12"/>
+      <c r="H681" s="15"/>
     </row>
     <row r="682" ht="14.25" customHeight="1">
-      <c r="H682" s="12"/>
+      <c r="H682" s="15"/>
     </row>
     <row r="683" ht="14.25" customHeight="1">
-      <c r="H683" s="12"/>
+      <c r="H683" s="15"/>
     </row>
     <row r="684" ht="14.25" customHeight="1">
-      <c r="H684" s="12"/>
+      <c r="H684" s="15"/>
     </row>
     <row r="685" ht="14.25" customHeight="1">
-      <c r="H685" s="12"/>
+      <c r="H685" s="15"/>
     </row>
     <row r="686" ht="14.25" customHeight="1">
-      <c r="H686" s="12"/>
+      <c r="H686" s="15"/>
     </row>
     <row r="687" ht="14.25" customHeight="1">
-      <c r="H687" s="12"/>
+      <c r="H687" s="15"/>
     </row>
     <row r="688" ht="14.25" customHeight="1">
-      <c r="H688" s="12"/>
+      <c r="H688" s="15"/>
     </row>
     <row r="689" ht="14.25" customHeight="1">
-      <c r="H689" s="12"/>
+      <c r="H689" s="15"/>
     </row>
     <row r="690" ht="14.25" customHeight="1">
-      <c r="H690" s="12"/>
+      <c r="H690" s="15"/>
     </row>
     <row r="691" ht="14.25" customHeight="1">
-      <c r="H691" s="12"/>
+      <c r="H691" s="15"/>
     </row>
     <row r="692" ht="14.25" customHeight="1">
-      <c r="H692" s="12"/>
+      <c r="H692" s="15"/>
     </row>
     <row r="693" ht="14.25" customHeight="1">
-      <c r="H693" s="12"/>
+      <c r="H693" s="15"/>
     </row>
     <row r="694" ht="14.25" customHeight="1">
-      <c r="H694" s="12"/>
+      <c r="H694" s="15"/>
     </row>
     <row r="695" ht="14.25" customHeight="1">
-      <c r="H695" s="12"/>
+      <c r="H695" s="15"/>
     </row>
     <row r="696" ht="14.25" customHeight="1">
-      <c r="H696" s="12"/>
+      <c r="H696" s="15"/>
     </row>
     <row r="697" ht="14.25" customHeight="1">
-      <c r="H697" s="12"/>
+      <c r="H697" s="15"/>
     </row>
     <row r="698" ht="14.25" customHeight="1">
-      <c r="H698" s="12"/>
+      <c r="H698" s="15"/>
     </row>
     <row r="699" ht="14.25" customHeight="1">
-      <c r="H699" s="12"/>
+      <c r="H699" s="15"/>
     </row>
     <row r="700" ht="14.25" customHeight="1">
-      <c r="H700" s="12"/>
+      <c r="H700" s="15"/>
     </row>
     <row r="701" ht="14.25" customHeight="1">
-      <c r="H701" s="12"/>
+      <c r="H701" s="15"/>
     </row>
     <row r="702" ht="14.25" customHeight="1">
-      <c r="H702" s="12"/>
+      <c r="H702" s="15"/>
     </row>
     <row r="703" ht="14.25" customHeight="1">
-      <c r="H703" s="12"/>
+      <c r="H703" s="15"/>
     </row>
     <row r="704" ht="14.25" customHeight="1">
-      <c r="H704" s="12"/>
+      <c r="H704" s="15"/>
     </row>
     <row r="705" ht="14.25" customHeight="1">
-      <c r="H705" s="12"/>
+      <c r="H705" s="15"/>
     </row>
     <row r="706" ht="14.25" customHeight="1">
-      <c r="H706" s="12"/>
+      <c r="H706" s="15"/>
     </row>
     <row r="707" ht="14.25" customHeight="1">
-      <c r="H707" s="12"/>
+      <c r="H707" s="15"/>
     </row>
     <row r="708" ht="14.25" customHeight="1">
-      <c r="H708" s="12"/>
+      <c r="H708" s="15"/>
     </row>
     <row r="709" ht="14.25" customHeight="1">
-      <c r="H709" s="12"/>
+      <c r="H709" s="15"/>
     </row>
     <row r="710" ht="14.25" customHeight="1">
-      <c r="H710" s="12"/>
+      <c r="H710" s="15"/>
     </row>
     <row r="711" ht="14.25" customHeight="1">
-      <c r="H711" s="12"/>
+      <c r="H711" s="15"/>
     </row>
     <row r="712" ht="14.25" customHeight="1">
-      <c r="H712" s="12"/>
+      <c r="H712" s="15"/>
     </row>
     <row r="713" ht="14.25" customHeight="1">
-      <c r="H713" s="12"/>
+      <c r="H713" s="15"/>
     </row>
     <row r="714" ht="14.25" customHeight="1">
-      <c r="H714" s="12"/>
+      <c r="H714" s="15"/>
     </row>
     <row r="715" ht="14.25" customHeight="1">
-      <c r="H715" s="12"/>
+      <c r="H715" s="15"/>
     </row>
     <row r="716" ht="14.25" customHeight="1">
-      <c r="H716" s="12"/>
+      <c r="H716" s="15"/>
     </row>
     <row r="717" ht="14.25" customHeight="1">
-      <c r="H717" s="12"/>
+      <c r="H717" s="15"/>
     </row>
     <row r="718" ht="14.25" customHeight="1">
-      <c r="H718" s="12"/>
+      <c r="H718" s="15"/>
     </row>
     <row r="719" ht="14.25" customHeight="1">
-      <c r="H719" s="12"/>
+      <c r="H719" s="15"/>
     </row>
     <row r="720" ht="14.25" customHeight="1">
-      <c r="H720" s="12"/>
+      <c r="H720" s="15"/>
     </row>
     <row r="721" ht="14.25" customHeight="1">
-      <c r="H721" s="12"/>
+      <c r="H721" s="15"/>
     </row>
     <row r="722" ht="14.25" customHeight="1">
-      <c r="H722" s="12"/>
+      <c r="H722" s="15"/>
     </row>
     <row r="723" ht="14.25" customHeight="1">
-      <c r="H723" s="12"/>
+      <c r="H723" s="15"/>
     </row>
     <row r="724" ht="14.25" customHeight="1">
-      <c r="H724" s="12"/>
+      <c r="H724" s="15"/>
     </row>
     <row r="725" ht="14.25" customHeight="1">
-      <c r="H725" s="12"/>
+      <c r="H725" s="15"/>
     </row>
     <row r="726" ht="14.25" customHeight="1">
-      <c r="H726" s="12"/>
+      <c r="H726" s="15"/>
     </row>
     <row r="727" ht="14.25" customHeight="1">
-      <c r="H727" s="12"/>
+      <c r="H727" s="15"/>
     </row>
     <row r="728" ht="14.25" customHeight="1">
-      <c r="H728" s="12"/>
+      <c r="H728" s="15"/>
     </row>
     <row r="729" ht="14.25" customHeight="1">
-      <c r="H729" s="12"/>
+      <c r="H729" s="15"/>
     </row>
     <row r="730" ht="14.25" customHeight="1">
-      <c r="H730" s="12"/>
+      <c r="H730" s="15"/>
     </row>
     <row r="731" ht="14.25" customHeight="1">
-      <c r="H731" s="12"/>
+      <c r="H731" s="15"/>
     </row>
     <row r="732" ht="14.25" customHeight="1">
-      <c r="H732" s="12"/>
+      <c r="H732" s="15"/>
     </row>
     <row r="733" ht="14.25" customHeight="1">
-      <c r="H733" s="12"/>
+      <c r="H733" s="15"/>
     </row>
     <row r="734" ht="14.25" customHeight="1">
-      <c r="H734" s="12"/>
+      <c r="H734" s="15"/>
     </row>
     <row r="735" ht="14.25" customHeight="1">
-      <c r="H735" s="12"/>
+      <c r="H735" s="15"/>
     </row>
     <row r="736" ht="14.25" customHeight="1">
-      <c r="H736" s="12"/>
+      <c r="H736" s="15"/>
     </row>
     <row r="737" ht="14.25" customHeight="1">
-      <c r="H737" s="12"/>
+      <c r="H737" s="15"/>
     </row>
     <row r="738" ht="14.25" customHeight="1">
-      <c r="H738" s="12"/>
+      <c r="H738" s="15"/>
     </row>
     <row r="739" ht="14.25" customHeight="1">
-      <c r="H739" s="12"/>
+      <c r="H739" s="15"/>
     </row>
     <row r="740" ht="14.25" customHeight="1">
-      <c r="H740" s="12"/>
+      <c r="H740" s="15"/>
     </row>
     <row r="741" ht="14.25" customHeight="1">
-      <c r="H741" s="12"/>
+      <c r="H741" s="15"/>
     </row>
     <row r="742" ht="14.25" customHeight="1">
-      <c r="H742" s="12"/>
+      <c r="H742" s="15"/>
     </row>
     <row r="743" ht="14.25" customHeight="1">
-      <c r="H743" s="12"/>
+      <c r="H743" s="15"/>
     </row>
     <row r="744" ht="14.25" customHeight="1">
-      <c r="H744" s="12"/>
+      <c r="H744" s="15"/>
     </row>
     <row r="745" ht="14.25" customHeight="1">
-      <c r="H745" s="12"/>
+      <c r="H745" s="15"/>
     </row>
     <row r="746" ht="14.25" customHeight="1">
-      <c r="H746" s="12"/>
+      <c r="H746" s="15"/>
     </row>
     <row r="747" ht="14.25" customHeight="1">
-      <c r="H747" s="12"/>
+      <c r="H747" s="15"/>
     </row>
     <row r="748" ht="14.25" customHeight="1">
-      <c r="H748" s="12"/>
+      <c r="H748" s="15"/>
     </row>
     <row r="749" ht="14.25" customHeight="1">
-      <c r="H749" s="12"/>
+      <c r="H749" s="15"/>
     </row>
     <row r="750" ht="14.25" customHeight="1">
-      <c r="H750" s="12"/>
+      <c r="H750" s="15"/>
     </row>
     <row r="751" ht="14.25" customHeight="1">
-      <c r="H751" s="12"/>
+      <c r="H751" s="15"/>
     </row>
     <row r="752" ht="14.25" customHeight="1">
-      <c r="H752" s="12"/>
+      <c r="H752" s="15"/>
     </row>
     <row r="753" ht="14.25" customHeight="1">
-      <c r="H753" s="12"/>
+      <c r="H753" s="15"/>
     </row>
     <row r="754" ht="14.25" customHeight="1">
-      <c r="H754" s="12"/>
+      <c r="H754" s="15"/>
     </row>
     <row r="755" ht="14.25" customHeight="1">
-      <c r="H755" s="12"/>
+      <c r="H755" s="15"/>
     </row>
     <row r="756" ht="14.25" customHeight="1">
-      <c r="H756" s="12"/>
+      <c r="H756" s="15"/>
     </row>
     <row r="757" ht="14.25" customHeight="1">
-      <c r="H757" s="12"/>
+      <c r="H757" s="15"/>
     </row>
     <row r="758" ht="14.25" customHeight="1">
-      <c r="H758" s="12"/>
+      <c r="H758" s="15"/>
     </row>
     <row r="759" ht="14.25" customHeight="1">
-      <c r="H759" s="12"/>
+      <c r="H759" s="15"/>
     </row>
     <row r="760" ht="14.25" customHeight="1">
-      <c r="H760" s="12"/>
+      <c r="H760" s="15"/>
     </row>
     <row r="761" ht="14.25" customHeight="1">
-      <c r="H761" s="12"/>
+      <c r="H761" s="15"/>
     </row>
     <row r="762" ht="14.25" customHeight="1">
-      <c r="H762" s="12"/>
+      <c r="H762" s="15"/>
     </row>
     <row r="763" ht="14.25" customHeight="1">
-      <c r="H763" s="12"/>
+      <c r="H763" s="15"/>
     </row>
     <row r="764" ht="14.25" customHeight="1">
-      <c r="H764" s="12"/>
+      <c r="H764" s="15"/>
     </row>
     <row r="765" ht="14.25" customHeight="1">
-      <c r="H765" s="12"/>
+      <c r="H765" s="15"/>
     </row>
     <row r="766" ht="14.25" customHeight="1">
-      <c r="H766" s="12"/>
+      <c r="H766" s="15"/>
     </row>
     <row r="767" ht="14.25" customHeight="1">
-      <c r="H767" s="12"/>
+      <c r="H767" s="15"/>
     </row>
     <row r="768" ht="14.25" customHeight="1">
-      <c r="H768" s="12"/>
+      <c r="H768" s="15"/>
     </row>
     <row r="769" ht="14.25" customHeight="1">
-      <c r="H769" s="12"/>
+      <c r="H769" s="15"/>
     </row>
     <row r="770" ht="14.25" customHeight="1">
-      <c r="H770" s="12"/>
+      <c r="H770" s="15"/>
     </row>
     <row r="771" ht="14.25" customHeight="1">
-      <c r="H771" s="12"/>
+      <c r="H771" s="15"/>
     </row>
     <row r="772" ht="14.25" customHeight="1">
-      <c r="H772" s="12"/>
+      <c r="H772" s="15"/>
     </row>
     <row r="773" ht="14.25" customHeight="1">
-      <c r="H773" s="12"/>
+      <c r="H773" s="15"/>
     </row>
     <row r="774" ht="14.25" customHeight="1">
-      <c r="H774" s="12"/>
+      <c r="H774" s="15"/>
     </row>
     <row r="775" ht="14.25" customHeight="1">
-      <c r="H775" s="12"/>
+      <c r="H775" s="15"/>
     </row>
     <row r="776" ht="14.25" customHeight="1">
-      <c r="H776" s="12"/>
+      <c r="H776" s="15"/>
     </row>
     <row r="777" ht="14.25" customHeight="1">
-      <c r="H777" s="12"/>
+      <c r="H777" s="15"/>
     </row>
     <row r="778" ht="14.25" customHeight="1">
-      <c r="H778" s="12"/>
+      <c r="H778" s="15"/>
     </row>
     <row r="779" ht="14.25" customHeight="1">
-      <c r="H779" s="12"/>
+      <c r="H779" s="15"/>
     </row>
     <row r="780" ht="14.25" customHeight="1">
-      <c r="H780" s="12"/>
+      <c r="H780" s="15"/>
     </row>
     <row r="781" ht="14.25" customHeight="1">
-      <c r="H781" s="12"/>
+      <c r="H781" s="15"/>
     </row>
     <row r="782" ht="14.25" customHeight="1">
-      <c r="H782" s="12"/>
+      <c r="H782" s="15"/>
     </row>
     <row r="783" ht="14.25" customHeight="1">
-      <c r="H783" s="12"/>
+      <c r="H783" s="15"/>
     </row>
     <row r="784" ht="14.25" customHeight="1">
-      <c r="H784" s="12"/>
+      <c r="H784" s="15"/>
     </row>
     <row r="785" ht="14.25" customHeight="1">
-      <c r="H785" s="12"/>
+      <c r="H785" s="15"/>
     </row>
     <row r="786" ht="14.25" customHeight="1">
-      <c r="H786" s="12"/>
+      <c r="H786" s="15"/>
     </row>
     <row r="787" ht="14.25" customHeight="1">
-      <c r="H787" s="12"/>
+      <c r="H787" s="15"/>
     </row>
     <row r="788" ht="14.25" customHeight="1">
-      <c r="H788" s="12"/>
+      <c r="H788" s="15"/>
     </row>
     <row r="789" ht="14.25" customHeight="1">
-      <c r="H789" s="12"/>
+      <c r="H789" s="15"/>
     </row>
     <row r="790" ht="14.25" customHeight="1">
-      <c r="H790" s="12"/>
+      <c r="H790" s="15"/>
     </row>
     <row r="791" ht="14.25" customHeight="1">
-      <c r="H791" s="12"/>
+      <c r="H791" s="15"/>
     </row>
     <row r="792" ht="14.25" customHeight="1">
-      <c r="H792" s="12"/>
+      <c r="H792" s="15"/>
     </row>
     <row r="793" ht="14.25" customHeight="1">
-      <c r="H793" s="12"/>
+      <c r="H793" s="15"/>
     </row>
     <row r="794" ht="14.25" customHeight="1">
-      <c r="H794" s="12"/>
+      <c r="H794" s="15"/>
     </row>
     <row r="795" ht="14.25" customHeight="1">
-      <c r="H795" s="12"/>
+      <c r="H795" s="15"/>
     </row>
     <row r="796" ht="14.25" customHeight="1">
-      <c r="H796" s="12"/>
+      <c r="H796" s="15"/>
     </row>
     <row r="797" ht="14.25" customHeight="1">
-      <c r="H797" s="12"/>
+      <c r="H797" s="15"/>
     </row>
     <row r="798" ht="14.25" customHeight="1">
-      <c r="H798" s="12"/>
+      <c r="H798" s="15"/>
     </row>
     <row r="799" ht="14.25" customHeight="1">
-      <c r="H799" s="12"/>
+      <c r="H799" s="15"/>
     </row>
     <row r="800" ht="14.25" customHeight="1">
-      <c r="H800" s="12"/>
+      <c r="H800" s="15"/>
     </row>
     <row r="801" ht="14.25" customHeight="1">
-      <c r="H801" s="12"/>
+      <c r="H801" s="15"/>
     </row>
     <row r="802" ht="14.25" customHeight="1">
-      <c r="H802" s="12"/>
+      <c r="H802" s="15"/>
     </row>
     <row r="803" ht="14.25" customHeight="1">
-      <c r="H803" s="12"/>
+      <c r="H803" s="15"/>
     </row>
     <row r="804" ht="14.25" customHeight="1">
-      <c r="H804" s="12"/>
+      <c r="H804" s="15"/>
     </row>
     <row r="805" ht="14.25" customHeight="1">
-      <c r="H805" s="12"/>
+      <c r="H805" s="15"/>
     </row>
     <row r="806" ht="14.25" customHeight="1">
-      <c r="H806" s="12"/>
+      <c r="H806" s="15"/>
     </row>
     <row r="807" ht="14.25" customHeight="1">
-      <c r="H807" s="12"/>
+      <c r="H807" s="15"/>
     </row>
     <row r="808" ht="14.25" customHeight="1">
-      <c r="H808" s="12"/>
+      <c r="H808" s="15"/>
     </row>
     <row r="809" ht="14.25" customHeight="1">
-      <c r="H809" s="12"/>
+      <c r="H809" s="15"/>
     </row>
     <row r="810" ht="14.25" customHeight="1">
-      <c r="H810" s="12"/>
+      <c r="H810" s="15"/>
     </row>
     <row r="811" ht="14.25" customHeight="1">
-      <c r="H811" s="12"/>
+      <c r="H811" s="15"/>
     </row>
     <row r="812" ht="14.25" customHeight="1">
-      <c r="H812" s="12"/>
+      <c r="H812" s="15"/>
     </row>
     <row r="813" ht="14.25" customHeight="1">
-      <c r="H813" s="12"/>
+      <c r="H813" s="15"/>
     </row>
     <row r="814" ht="14.25" customHeight="1">
-      <c r="H814" s="12"/>
+      <c r="H814" s="15"/>
     </row>
     <row r="815" ht="14.25" customHeight="1">
-      <c r="H815" s="12"/>
+      <c r="H815" s="15"/>
     </row>
     <row r="816" ht="14.25" customHeight="1">
-      <c r="H816" s="12"/>
+      <c r="H816" s="15"/>
     </row>
     <row r="817" ht="14.25" customHeight="1">
-      <c r="H817" s="12"/>
+      <c r="H817" s="15"/>
     </row>
     <row r="818" ht="14.25" customHeight="1">
-      <c r="H818" s="12"/>
+      <c r="H818" s="15"/>
     </row>
     <row r="819" ht="14.25" customHeight="1">
-      <c r="H819" s="12"/>
+      <c r="H819" s="15"/>
     </row>
     <row r="820" ht="14.25" customHeight="1">
-      <c r="H820" s="12"/>
+      <c r="H820" s="15"/>
     </row>
     <row r="821" ht="14.25" customHeight="1">
-      <c r="H821" s="12"/>
+      <c r="H821" s="15"/>
     </row>
     <row r="822" ht="14.25" customHeight="1">
-      <c r="H822" s="12"/>
+      <c r="H822" s="15"/>
     </row>
     <row r="823" ht="14.25" customHeight="1">
-      <c r="H823" s="12"/>
+      <c r="H823" s="15"/>
     </row>
     <row r="824" ht="14.25" customHeight="1">
-      <c r="H824" s="12"/>
+      <c r="H824" s="15"/>
     </row>
     <row r="825" ht="14.25" customHeight="1">
-      <c r="H825" s="12"/>
+      <c r="H825" s="15"/>
     </row>
     <row r="826" ht="14.25" customHeight="1">
-      <c r="H826" s="12"/>
+      <c r="H826" s="15"/>
     </row>
     <row r="827" ht="14.25" customHeight="1">
-      <c r="H827" s="12"/>
+      <c r="H827" s="15"/>
     </row>
     <row r="828" ht="14.25" customHeight="1">
-      <c r="H828" s="12"/>
+      <c r="H828" s="15"/>
     </row>
     <row r="829" ht="14.25" customHeight="1">
-      <c r="H829" s="12"/>
+      <c r="H829" s="15"/>
     </row>
     <row r="830" ht="14.25" customHeight="1">
-      <c r="H830" s="12"/>
+      <c r="H830" s="15"/>
     </row>
     <row r="831" ht="14.25" customHeight="1">
-      <c r="H831" s="12"/>
+      <c r="H831" s="15"/>
     </row>
     <row r="832" ht="14.25" customHeight="1">
-      <c r="H832" s="12"/>
+      <c r="H832" s="15"/>
     </row>
     <row r="833" ht="14.25" customHeight="1">
-      <c r="H833" s="12"/>
+      <c r="H833" s="15"/>
     </row>
     <row r="834" ht="14.25" customHeight="1">
-      <c r="H834" s="12"/>
+      <c r="H834" s="15"/>
     </row>
     <row r="835" ht="14.25" customHeight="1">
-      <c r="H835" s="12"/>
+      <c r="H835" s="15"/>
     </row>
     <row r="836" ht="14.25" customHeight="1">
-      <c r="H836" s="12"/>
+      <c r="H836" s="15"/>
     </row>
     <row r="837" ht="14.25" customHeight="1">
-      <c r="H837" s="12"/>
+      <c r="H837" s="15"/>
     </row>
     <row r="838" ht="14.25" customHeight="1">
-      <c r="H838" s="12"/>
+      <c r="H838" s="15"/>
     </row>
     <row r="839" ht="14.25" customHeight="1">
-      <c r="H839" s="12"/>
+      <c r="H839" s="15"/>
     </row>
     <row r="840" ht="14.25" customHeight="1">
-      <c r="H840" s="12"/>
+      <c r="H840" s="15"/>
     </row>
     <row r="841" ht="14.25" customHeight="1">
-      <c r="H841" s="12"/>
+      <c r="H841" s="15"/>
     </row>
     <row r="842" ht="14.25" customHeight="1">
-      <c r="H842" s="12"/>
+      <c r="H842" s="15"/>
     </row>
     <row r="843" ht="14.25" customHeight="1">
-      <c r="H843" s="12"/>
+      <c r="H843" s="15"/>
     </row>
     <row r="844" ht="14.25" customHeight="1">
-      <c r="H844" s="12"/>
+      <c r="H844" s="15"/>
     </row>
     <row r="845" ht="14.25" customHeight="1">
-      <c r="H845" s="12"/>
+      <c r="H845" s="15"/>
     </row>
     <row r="846" ht="14.25" customHeight="1">
-      <c r="H846" s="12"/>
+      <c r="H846" s="15"/>
     </row>
     <row r="847" ht="14.25" customHeight="1">
-      <c r="H847" s="12"/>
+      <c r="H847" s="15"/>
     </row>
     <row r="848" ht="14.25" customHeight="1">
-      <c r="H848" s="12"/>
+      <c r="H848" s="15"/>
     </row>
     <row r="849" ht="14.25" customHeight="1">
-      <c r="H849" s="12"/>
+      <c r="H849" s="15"/>
     </row>
     <row r="850" ht="14.25" customHeight="1">
-      <c r="H850" s="12"/>
+      <c r="H850" s="15"/>
     </row>
     <row r="851" ht="14.25" customHeight="1">
-      <c r="H851" s="12"/>
+      <c r="H851" s="15"/>
     </row>
     <row r="852" ht="14.25" customHeight="1">
-      <c r="H852" s="12"/>
+      <c r="H852" s="15"/>
     </row>
     <row r="853" ht="14.25" customHeight="1">
-      <c r="H853" s="12"/>
+      <c r="H853" s="15"/>
     </row>
     <row r="854" ht="14.25" customHeight="1">
-      <c r="H854" s="12"/>
+      <c r="H854" s="15"/>
     </row>
     <row r="855" ht="14.25" customHeight="1">
-      <c r="H855" s="12"/>
+      <c r="H855" s="15"/>
     </row>
     <row r="856" ht="14.25" customHeight="1">
-      <c r="H856" s="12"/>
+      <c r="H856" s="15"/>
     </row>
     <row r="857" ht="14.25" customHeight="1">
-      <c r="H857" s="12"/>
+      <c r="H857" s="15"/>
     </row>
     <row r="858" ht="14.25" customHeight="1">
-      <c r="H858" s="12"/>
+      <c r="H858" s="15"/>
     </row>
     <row r="859" ht="14.25" customHeight="1">
-      <c r="H859" s="12"/>
+      <c r="H859" s="15"/>
     </row>
     <row r="860" ht="14.25" customHeight="1">
-      <c r="H860" s="12"/>
+      <c r="H860" s="15"/>
     </row>
     <row r="861" ht="14.25" customHeight="1">
-      <c r="H861" s="12"/>
+      <c r="H861" s="15"/>
     </row>
     <row r="862" ht="14.25" customHeight="1">
-      <c r="H862" s="12"/>
+      <c r="H862" s="15"/>
     </row>
     <row r="863" ht="14.25" customHeight="1">
-      <c r="H863" s="12"/>
+      <c r="H863" s="15"/>
     </row>
     <row r="864" ht="14.25" customHeight="1">
-      <c r="H864" s="12"/>
+      <c r="H864" s="15"/>
     </row>
     <row r="865" ht="14.25" customHeight="1">
-      <c r="H865" s="12"/>
+      <c r="H865" s="15"/>
     </row>
     <row r="866" ht="14.25" customHeight="1">
-      <c r="H866" s="12"/>
+      <c r="H866" s="15"/>
     </row>
     <row r="867" ht="14.25" customHeight="1">
-      <c r="H867" s="12"/>
+      <c r="H867" s="15"/>
     </row>
     <row r="868" ht="14.25" customHeight="1">
-      <c r="H868" s="12"/>
+      <c r="H868" s="15"/>
     </row>
     <row r="869" ht="14.25" customHeight="1">
-      <c r="H869" s="12"/>
+      <c r="H869" s="15"/>
     </row>
     <row r="870" ht="14.25" customHeight="1">
-      <c r="H870" s="12"/>
+      <c r="H870" s="15"/>
     </row>
     <row r="871" ht="14.25" customHeight="1">
-      <c r="H871" s="12"/>
+      <c r="H871" s="15"/>
     </row>
     <row r="872" ht="14.25" customHeight="1">
-      <c r="H872" s="12"/>
+      <c r="H872" s="15"/>
     </row>
     <row r="873" ht="14.25" customHeight="1">
-      <c r="H873" s="12"/>
+      <c r="H873" s="15"/>
     </row>
     <row r="874" ht="14.25" customHeight="1">
-      <c r="H874" s="12"/>
+      <c r="H874" s="15"/>
     </row>
     <row r="875" ht="14.25" customHeight="1">
-      <c r="H875" s="12"/>
+      <c r="H875" s="15"/>
     </row>
     <row r="876" ht="14.25" customHeight="1">
-      <c r="H876" s="12"/>
+      <c r="H876" s="15"/>
     </row>
     <row r="877" ht="14.25" customHeight="1">
-      <c r="H877" s="12"/>
+      <c r="H877" s="15"/>
     </row>
     <row r="878" ht="14.25" customHeight="1">
-      <c r="H878" s="12"/>
+      <c r="H878" s="15"/>
     </row>
     <row r="879" ht="14.25" customHeight="1">
-      <c r="H879" s="12"/>
+      <c r="H879" s="15"/>
     </row>
     <row r="880" ht="14.25" customHeight="1">
-      <c r="H880" s="12"/>
+      <c r="H880" s="15"/>
     </row>
     <row r="881" ht="14.25" customHeight="1">
-      <c r="H881" s="12"/>
+      <c r="H881" s="15"/>
     </row>
     <row r="882" ht="14.25" customHeight="1">
-      <c r="H882" s="12"/>
+      <c r="H882" s="15"/>
     </row>
     <row r="883" ht="14.25" customHeight="1">
-      <c r="H883" s="12"/>
+      <c r="H883" s="15"/>
     </row>
     <row r="884" ht="14.25" customHeight="1">
-      <c r="H884" s="12"/>
+      <c r="H884" s="15"/>
     </row>
     <row r="885" ht="14.25" customHeight="1">
-      <c r="H885" s="12"/>
+      <c r="H885" s="15"/>
     </row>
     <row r="886" ht="14.25" customHeight="1">
-      <c r="H886" s="12"/>
+      <c r="H886" s="15"/>
     </row>
     <row r="887" ht="14.25" customHeight="1">
-      <c r="H887" s="12"/>
+      <c r="H887" s="15"/>
     </row>
     <row r="888" ht="14.25" customHeight="1">
-      <c r="H888" s="12"/>
+      <c r="H888" s="15"/>
     </row>
     <row r="889" ht="14.25" customHeight="1">
-      <c r="H889" s="12"/>
+      <c r="H889" s="15"/>
     </row>
     <row r="890" ht="14.25" customHeight="1">
-      <c r="H890" s="12"/>
+      <c r="H890" s="15"/>
     </row>
     <row r="891" ht="14.25" customHeight="1">
-      <c r="H891" s="12"/>
+      <c r="H891" s="15"/>
     </row>
     <row r="892" ht="14.25" customHeight="1">
-      <c r="H892" s="12"/>
+      <c r="H892" s="15"/>
     </row>
     <row r="893" ht="14.25" customHeight="1">
-      <c r="H893" s="12"/>
+      <c r="H893" s="15"/>
     </row>
     <row r="894" ht="14.25" customHeight="1">
-      <c r="H894" s="12"/>
+      <c r="H894" s="15"/>
     </row>
     <row r="895" ht="14.25" customHeight="1">
-      <c r="H895" s="12"/>
+      <c r="H895" s="15"/>
     </row>
     <row r="896" ht="14.25" customHeight="1">
-      <c r="H896" s="12"/>
+      <c r="H896" s="15"/>
     </row>
     <row r="897" ht="14.25" customHeight="1">
-      <c r="H897" s="12"/>
+      <c r="H897" s="15"/>
     </row>
     <row r="898" ht="14.25" customHeight="1">
-      <c r="H898" s="12"/>
+      <c r="H898" s="15"/>
     </row>
     <row r="899" ht="14.25" customHeight="1">
-      <c r="H899" s="12"/>
+      <c r="H899" s="15"/>
     </row>
     <row r="900" ht="14.25" customHeight="1">
-      <c r="H900" s="12"/>
+      <c r="H900" s="15"/>
     </row>
     <row r="901" ht="14.25" customHeight="1">
-      <c r="H901" s="12"/>
+      <c r="H901" s="15"/>
     </row>
     <row r="902" ht="14.25" customHeight="1">
-      <c r="H902" s="12"/>
+      <c r="H902" s="15"/>
     </row>
     <row r="903" ht="14.25" customHeight="1">
-      <c r="H903" s="12"/>
+      <c r="H903" s="15"/>
     </row>
     <row r="904" ht="14.25" customHeight="1">
-      <c r="H904" s="12"/>
+      <c r="H904" s="15"/>
     </row>
     <row r="905" ht="14.25" customHeight="1">
-      <c r="H905" s="12"/>
+      <c r="H905" s="15"/>
     </row>
     <row r="906" ht="14.25" customHeight="1">
-      <c r="H906" s="12"/>
+      <c r="H906" s="15"/>
     </row>
     <row r="907" ht="14.25" customHeight="1">
-      <c r="H907" s="12"/>
+      <c r="H907" s="15"/>
     </row>
     <row r="908" ht="14.25" customHeight="1">
-      <c r="H908" s="12"/>
+      <c r="H908" s="15"/>
     </row>
     <row r="909" ht="14.25" customHeight="1">
-      <c r="H909" s="12"/>
+      <c r="H909" s="15"/>
     </row>
     <row r="910" ht="14.25" customHeight="1">
-      <c r="H910" s="12"/>
+      <c r="H910" s="15"/>
     </row>
     <row r="911" ht="14.25" customHeight="1">
-      <c r="H911" s="12"/>
+      <c r="H911" s="15"/>
     </row>
     <row r="912" ht="14.25" customHeight="1">
-      <c r="H912" s="12"/>
+      <c r="H912" s="15"/>
     </row>
     <row r="913" ht="14.25" customHeight="1">
-      <c r="H913" s="12"/>
+      <c r="H913" s="15"/>
     </row>
     <row r="914" ht="14.25" customHeight="1">
-      <c r="H914" s="12"/>
+      <c r="H914" s="15"/>
     </row>
     <row r="915" ht="14.25" customHeight="1">
-      <c r="H915" s="12"/>
+      <c r="H915" s="15"/>
     </row>
     <row r="916" ht="14.25" customHeight="1">
-      <c r="H916" s="12"/>
+      <c r="H916" s="15"/>
     </row>
     <row r="917" ht="14.25" customHeight="1">
-      <c r="H917" s="12"/>
+      <c r="H917" s="15"/>
     </row>
     <row r="918" ht="14.25" customHeight="1">
-      <c r="H918" s="12"/>
+      <c r="H918" s="15"/>
     </row>
     <row r="919" ht="14.25" customHeight="1">
-      <c r="H919" s="12"/>
+      <c r="H919" s="15"/>
     </row>
     <row r="920" ht="14.25" customHeight="1">
-      <c r="H920" s="12"/>
+      <c r="H920" s="15"/>
     </row>
     <row r="921" ht="14.25" customHeight="1">
-      <c r="H921" s="12"/>
+      <c r="H921" s="15"/>
     </row>
     <row r="922" ht="14.25" customHeight="1">
-      <c r="H922" s="12"/>
+      <c r="H922" s="15"/>
     </row>
     <row r="923" ht="14.25" customHeight="1">
-      <c r="H923" s="12"/>
+      <c r="H923" s="15"/>
     </row>
     <row r="924" ht="14.25" customHeight="1">
-      <c r="H924" s="12"/>
+      <c r="H924" s="15"/>
     </row>
     <row r="925" ht="14.25" customHeight="1">
-      <c r="H925" s="12"/>
+      <c r="H925" s="15"/>
     </row>
     <row r="926" ht="14.25" customHeight="1">
-      <c r="H926" s="12"/>
+      <c r="H926" s="15"/>
     </row>
     <row r="927" ht="14.25" customHeight="1">
-      <c r="H927" s="12"/>
+      <c r="H927" s="15"/>
     </row>
     <row r="928" ht="14.25" customHeight="1">
-      <c r="H928" s="12"/>
+      <c r="H928" s="15"/>
     </row>
     <row r="929" ht="14.25" customHeight="1">
-      <c r="H929" s="12"/>
+      <c r="H929" s="15"/>
     </row>
     <row r="930" ht="14.25" customHeight="1">
-      <c r="H930" s="12"/>
+      <c r="H930" s="15"/>
     </row>
     <row r="931" ht="14.25" customHeight="1">
-      <c r="H931" s="12"/>
+      <c r="H931" s="15"/>
     </row>
     <row r="932" ht="14.25" customHeight="1">
-      <c r="H932" s="12"/>
+      <c r="H932" s="15"/>
     </row>
     <row r="933" ht="14.25" customHeight="1">
-      <c r="H933" s="12"/>
+      <c r="H933" s="15"/>
     </row>
     <row r="934" ht="14.25" customHeight="1">
-      <c r="H934" s="12"/>
+      <c r="H934" s="15"/>
     </row>
     <row r="935" ht="14.25" customHeight="1">
-      <c r="H935" s="12"/>
+      <c r="H935" s="15"/>
     </row>
     <row r="936" ht="14.25" customHeight="1">
-      <c r="H936" s="12"/>
+      <c r="H936" s="15"/>
     </row>
     <row r="937" ht="14.25" customHeight="1">
-      <c r="H937" s="12"/>
+      <c r="H937" s="15"/>
     </row>
     <row r="938" ht="14.25" customHeight="1">
-      <c r="H938" s="12"/>
+      <c r="H938" s="15"/>
     </row>
     <row r="939" ht="14.25" customHeight="1">
-      <c r="H939" s="12"/>
+      <c r="H939" s="15"/>
     </row>
     <row r="940" ht="14.25" customHeight="1">
-      <c r="H940" s="12"/>
+      <c r="H940" s="15"/>
     </row>
     <row r="941" ht="14.25" customHeight="1">
-      <c r="H941" s="12"/>
+      <c r="H941" s="15"/>
     </row>
     <row r="942" ht="14.25" customHeight="1">
-      <c r="H942" s="12"/>
+      <c r="H942" s="15"/>
     </row>
     <row r="943" ht="14.25" customHeight="1">
-      <c r="H943" s="12"/>
+      <c r="H943" s="15"/>
     </row>
     <row r="944" ht="14.25" customHeight="1">
-      <c r="H944" s="12"/>
+      <c r="H944" s="15"/>
     </row>
     <row r="945" ht="14.25" customHeight="1">
-      <c r="H945" s="12"/>
+      <c r="H945" s="15"/>
     </row>
     <row r="946" ht="14.25" customHeight="1">
-      <c r="H946" s="12"/>
+      <c r="H946" s="15"/>
     </row>
     <row r="947" ht="14.25" customHeight="1">
-      <c r="H947" s="12"/>
+      <c r="H947" s="15"/>
     </row>
     <row r="948" ht="14.25" customHeight="1">
-      <c r="H948" s="12"/>
+      <c r="H948" s="15"/>
     </row>
     <row r="949" ht="14.25" customHeight="1">
-      <c r="H949" s="12"/>
+      <c r="H949" s="15"/>
     </row>
     <row r="950" ht="14.25" customHeight="1">
-      <c r="H950" s="12"/>
+      <c r="H950" s="15"/>
     </row>
     <row r="951" ht="14.25" customHeight="1">
-      <c r="H951" s="12"/>
+      <c r="H951" s="15"/>
     </row>
     <row r="952" ht="14.25" customHeight="1">
-      <c r="H952" s="12"/>
+      <c r="H952" s="15"/>
     </row>
     <row r="953" ht="14.25" customHeight="1">
-      <c r="H953" s="12"/>
+      <c r="H953" s="15"/>
     </row>
     <row r="954" ht="14.25" customHeight="1">
-      <c r="H954" s="12"/>
+      <c r="H954" s="15"/>
     </row>
     <row r="955" ht="14.25" customHeight="1">
-      <c r="H955" s="12"/>
+      <c r="H955" s="15"/>
     </row>
     <row r="956" ht="14.25" customHeight="1">
-      <c r="H956" s="12"/>
+      <c r="H956" s="15"/>
     </row>
     <row r="957" ht="14.25" customHeight="1">
-      <c r="H957" s="12"/>
+      <c r="H957" s="15"/>
     </row>
     <row r="958" ht="14.25" customHeight="1">
-      <c r="H958" s="12"/>
+      <c r="H958" s="15"/>
     </row>
     <row r="959" ht="14.25" customHeight="1">
-      <c r="H959" s="12"/>
+      <c r="H959" s="15"/>
     </row>
     <row r="960" ht="14.25" customHeight="1">
-      <c r="H960" s="12"/>
+      <c r="H960" s="15"/>
     </row>
     <row r="961" ht="14.25" customHeight="1">
-      <c r="H961" s="12"/>
+      <c r="H961" s="15"/>
     </row>
     <row r="962" ht="14.25" customHeight="1">
-      <c r="H962" s="12"/>
+      <c r="H962" s="15"/>
     </row>
     <row r="963" ht="14.25" customHeight="1">
-      <c r="H963" s="12"/>
+      <c r="H963" s="15"/>
     </row>
     <row r="964" ht="14.25" customHeight="1">
-      <c r="H964" s="12"/>
+      <c r="H964" s="15"/>
     </row>
     <row r="965" ht="14.25" customHeight="1">
-      <c r="H965" s="12"/>
+      <c r="H965" s="15"/>
     </row>
     <row r="966" ht="14.25" customHeight="1">
-      <c r="H966" s="12"/>
+      <c r="H966" s="15"/>
     </row>
     <row r="967" ht="14.25" customHeight="1">
-      <c r="H967" s="12"/>
+      <c r="H967" s="15"/>
     </row>
     <row r="968" ht="14.25" customHeight="1">
-      <c r="H968" s="12"/>
+      <c r="H968" s="15"/>
     </row>
     <row r="969" ht="14.25" customHeight="1">
-      <c r="H969" s="12"/>
+      <c r="H969" s="15"/>
     </row>
     <row r="970" ht="14.25" customHeight="1">
-      <c r="H970" s="12"/>
+      <c r="H970" s="15"/>
     </row>
     <row r="971" ht="14.25" customHeight="1">
-      <c r="H971" s="12"/>
+      <c r="H971" s="15"/>
     </row>
     <row r="972" ht="14.25" customHeight="1">
-      <c r="H972" s="12"/>
+      <c r="H972" s="15"/>
     </row>
     <row r="973" ht="14.25" customHeight="1">
-      <c r="H973" s="12"/>
+      <c r="H973" s="15"/>
     </row>
     <row r="974" ht="14.25" customHeight="1">
-      <c r="H974" s="12"/>
+      <c r="H974" s="15"/>
     </row>
     <row r="975" ht="14.25" customHeight="1">
-      <c r="H975" s="12"/>
+      <c r="H975" s="15"/>
     </row>
     <row r="976" ht="14.25" customHeight="1">
-      <c r="H976" s="12"/>
+      <c r="H976" s="15"/>
     </row>
     <row r="977" ht="14.25" customHeight="1">
-      <c r="H977" s="12"/>
+      <c r="H977" s="15"/>
     </row>
     <row r="978" ht="14.25" customHeight="1">
-      <c r="H978" s="12"/>
+      <c r="H978" s="15"/>
     </row>
     <row r="979" ht="14.25" customHeight="1">
-      <c r="H979" s="12"/>
+      <c r="H979" s="15"/>
     </row>
     <row r="980" ht="14.25" customHeight="1">
-      <c r="H980" s="12"/>
+      <c r="H980" s="15"/>
     </row>
     <row r="981" ht="14.25" customHeight="1">
-      <c r="H981" s="12"/>
+      <c r="H981" s="15"/>
     </row>
     <row r="982" ht="14.25" customHeight="1">
-      <c r="H982" s="12"/>
+      <c r="H982" s="15"/>
     </row>
     <row r="983" ht="14.25" customHeight="1">
-      <c r="H983" s="12"/>
+      <c r="H983" s="15"/>
     </row>
     <row r="984" ht="14.25" customHeight="1">
-      <c r="H984" s="12"/>
+      <c r="H984" s="15"/>
     </row>
     <row r="985" ht="14.25" customHeight="1">
-      <c r="H985" s="12"/>
+      <c r="H985" s="15"/>
     </row>
     <row r="986" ht="14.25" customHeight="1">
-      <c r="H986" s="12"/>
+      <c r="H986" s="15"/>
     </row>
     <row r="987" ht="14.25" customHeight="1">
-      <c r="H987" s="12"/>
+      <c r="H987" s="15"/>
     </row>
     <row r="988" ht="14.25" customHeight="1">
-      <c r="H988" s="12"/>
+      <c r="H988" s="15"/>
     </row>
     <row r="989" ht="14.25" customHeight="1">
-      <c r="H989" s="12"/>
+      <c r="H989" s="15"/>
     </row>
     <row r="990" ht="14.25" customHeight="1">
-      <c r="H990" s="12"/>
+      <c r="H990" s="15"/>
     </row>
     <row r="991" ht="14.25" customHeight="1">
-      <c r="H991" s="12"/>
+      <c r="H991" s="15"/>
     </row>
     <row r="992" ht="14.25" customHeight="1">
-      <c r="H992" s="12"/>
+      <c r="H992" s="15"/>
     </row>
     <row r="993" ht="14.25" customHeight="1">
-      <c r="H993" s="12"/>
+      <c r="H993" s="15"/>
     </row>
     <row r="994" ht="14.25" customHeight="1">
-      <c r="H994" s="12"/>
+      <c r="H994" s="15"/>
     </row>
     <row r="995" ht="14.25" customHeight="1">
-      <c r="H995" s="12"/>
+      <c r="H995" s="15"/>
     </row>
     <row r="996" ht="14.25" customHeight="1">
-      <c r="H996" s="12"/>
+      <c r="H996" s="15"/>
     </row>
     <row r="997" ht="14.25" customHeight="1">
-      <c r="H997" s="12"/>
+      <c r="H997" s="15"/>
     </row>
     <row r="998" ht="14.25" customHeight="1">
-      <c r="H998" s="12"/>
+      <c r="H998" s="15"/>
     </row>
     <row r="999" ht="14.25" customHeight="1">
-      <c r="H999" s="12"/>
+      <c r="H999" s="15"/>
     </row>
     <row r="1000" ht="14.25" customHeight="1">
-      <c r="H1000" s="12"/>
+      <c r="H1000" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="$B$6:$I$114"/>

</xml_diff>